<commit_message>
selected all seasons in the excel file.  Early spring was not selected before
</commit_message>
<xml_diff>
--- a/data/CANONICAL Bouquet Recipe Master Sheet.xlsx
+++ b/data/CANONICAL Bouquet Recipe Master Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Documents/Sweet Piedmont/Offerings/Software and Code/bouquet-blueprint-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CA9CD1-61F7-7344-B05B-84FD8AE8B42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BF66D1-B218-1F4B-BC8A-44F126336188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5060" yWindow="760" windowWidth="29500" windowHeight="21580" firstSheet="1" activeTab="1" xr2:uid="{835A2F5B-2282-E345-9D43-16C3FBECA701}"/>
   </bookViews>
@@ -11492,20 +11492,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{63FB889B-362F-FA4D-9D4D-A49BD91E0CC2}" name="Table31615" displayName="Table31615" ref="A1:J246" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141" tableBorderDxfId="140" headerRowCellStyle="Currency" dataCellStyle="Currency">
-  <autoFilter ref="A1:J246" xr:uid="{63FB889B-362F-FA4D-9D4D-A49BD91E0CC2}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Early Spring, Fall"/>
-        <filter val="Early Spring, Late Spring, Fall"/>
-        <filter val="Early Spring, Late Spring, Summer, Fall"/>
-        <filter val="Late Spring, Fall, Summer"/>
-        <filter val="Late Spring, Summer"/>
-        <filter val="Late Spring, Summer, Fall"/>
-        <filter val="Summer"/>
-        <filter val="Summer, Fall"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J246" xr:uid="{63FB889B-362F-FA4D-9D4D-A49BD91E0CC2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J246">
     <sortCondition ref="B1:B246"/>
   </sortState>
@@ -33243,8 +33230,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B247" sqref="B247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -33315,7 +33302,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -33341,7 +33328,7 @@
       <c r="I2" s="140"/>
       <c r="J2" s="140"/>
     </row>
-    <row r="3" spans="1:20" hidden="1">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -33367,7 +33354,7 @@
       <c r="I3" s="140"/>
       <c r="J3" s="140"/>
     </row>
-    <row r="4" spans="1:20" hidden="1">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -33393,7 +33380,7 @@
       <c r="I4" s="140"/>
       <c r="J4" s="140"/>
     </row>
-    <row r="5" spans="1:20" hidden="1">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -33419,7 +33406,7 @@
       <c r="I5" s="140"/>
       <c r="J5" s="140"/>
     </row>
-    <row r="6" spans="1:20" hidden="1">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -33445,7 +33432,7 @@
       <c r="I6" s="140"/>
       <c r="J6" s="140"/>
     </row>
-    <row r="7" spans="1:20" hidden="1">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -33473,7 +33460,7 @@
       <c r="I7" s="140"/>
       <c r="J7" s="140"/>
     </row>
-    <row r="8" spans="1:20" hidden="1">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -33500,7 +33487,7 @@
       <c r="I8" s="140"/>
       <c r="J8" s="140"/>
     </row>
-    <row r="9" spans="1:20" hidden="1">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -33526,7 +33513,7 @@
       <c r="I9" s="140"/>
       <c r="J9" s="140"/>
     </row>
-    <row r="10" spans="1:20" hidden="1">
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -33552,7 +33539,7 @@
       <c r="I10" s="140"/>
       <c r="J10" s="140"/>
     </row>
-    <row r="11" spans="1:20" hidden="1">
+    <row r="11" spans="1:20">
       <c r="A11" s="156" t="s">
         <v>22</v>
       </c>
@@ -33578,7 +33565,7 @@
       <c r="I11" s="140"/>
       <c r="J11" s="140"/>
     </row>
-    <row r="12" spans="1:20" hidden="1">
+    <row r="12" spans="1:20">
       <c r="A12" s="156" t="s">
         <v>22</v>
       </c>
@@ -33631,7 +33618,7 @@
       <c r="J13" s="140"/>
       <c r="K13" s="84"/>
     </row>
-    <row r="14" spans="1:20" hidden="1">
+    <row r="14" spans="1:20">
       <c r="A14" s="156" t="s">
         <v>31</v>
       </c>
@@ -33657,7 +33644,7 @@
       <c r="I14" s="140"/>
       <c r="J14" s="140"/>
     </row>
-    <row r="15" spans="1:20" hidden="1">
+    <row r="15" spans="1:20">
       <c r="A15" s="156" t="s">
         <v>31</v>
       </c>
@@ -33683,7 +33670,7 @@
       <c r="I15" s="140"/>
       <c r="J15" s="140"/>
     </row>
-    <row r="16" spans="1:20" hidden="1">
+    <row r="16" spans="1:20">
       <c r="A16" s="156" t="s">
         <v>31</v>
       </c>
@@ -33713,7 +33700,7 @@
       <c r="I16" s="140"/>
       <c r="J16" s="140"/>
     </row>
-    <row r="17" spans="1:10" hidden="1">
+    <row r="17" spans="1:10">
       <c r="A17" s="156" t="s">
         <v>31</v>
       </c>
@@ -33739,7 +33726,7 @@
       <c r="I17" s="140"/>
       <c r="J17" s="140"/>
     </row>
-    <row r="18" spans="1:10" hidden="1">
+    <row r="18" spans="1:10">
       <c r="A18" s="156" t="s">
         <v>31</v>
       </c>
@@ -33767,7 +33754,7 @@
       <c r="I18" s="140"/>
       <c r="J18" s="140"/>
     </row>
-    <row r="19" spans="1:10" hidden="1">
+    <row r="19" spans="1:10">
       <c r="A19" s="156" t="s">
         <v>31</v>
       </c>
@@ -33793,7 +33780,7 @@
       <c r="I19" s="140"/>
       <c r="J19" s="140"/>
     </row>
-    <row r="20" spans="1:10" hidden="1">
+    <row r="20" spans="1:10">
       <c r="A20" s="156" t="s">
         <v>31</v>
       </c>
@@ -33819,7 +33806,7 @@
       <c r="I20" s="140"/>
       <c r="J20" s="140"/>
     </row>
-    <row r="21" spans="1:10" hidden="1">
+    <row r="21" spans="1:10">
       <c r="A21" s="156" t="s">
         <v>31</v>
       </c>
@@ -33897,7 +33884,7 @@
       <c r="I23" s="140"/>
       <c r="J23" s="140"/>
     </row>
-    <row r="24" spans="1:10" hidden="1">
+    <row r="24" spans="1:10">
       <c r="A24" s="156" t="s">
         <v>22</v>
       </c>
@@ -33923,7 +33910,7 @@
       <c r="I24" s="140"/>
       <c r="J24" s="140"/>
     </row>
-    <row r="25" spans="1:10" hidden="1">
+    <row r="25" spans="1:10">
       <c r="A25" s="156" t="s">
         <v>22</v>
       </c>
@@ -33949,7 +33936,7 @@
       <c r="I25" s="140"/>
       <c r="J25" s="140"/>
     </row>
-    <row r="26" spans="1:10" hidden="1">
+    <row r="26" spans="1:10">
       <c r="A26" s="156" t="s">
         <v>31</v>
       </c>
@@ -34001,7 +33988,7 @@
       <c r="I27" s="140"/>
       <c r="J27" s="140"/>
     </row>
-    <row r="28" spans="1:10" hidden="1">
+    <row r="28" spans="1:10">
       <c r="A28" s="156" t="s">
         <v>58</v>
       </c>
@@ -34027,7 +34014,7 @@
       <c r="I28" s="140"/>
       <c r="J28" s="140"/>
     </row>
-    <row r="29" spans="1:10" hidden="1">
+    <row r="29" spans="1:10">
       <c r="A29" s="156" t="s">
         <v>58</v>
       </c>
@@ -34055,7 +34042,7 @@
       <c r="I29" s="140"/>
       <c r="J29" s="140"/>
     </row>
-    <row r="30" spans="1:10" hidden="1">
+    <row r="30" spans="1:10">
       <c r="A30" s="156" t="s">
         <v>58</v>
       </c>
@@ -34083,7 +34070,7 @@
       <c r="I30" s="140"/>
       <c r="J30" s="140"/>
     </row>
-    <row r="31" spans="1:10" hidden="1">
+    <row r="31" spans="1:10">
       <c r="A31" s="156" t="s">
         <v>58</v>
       </c>
@@ -34109,7 +34096,7 @@
       <c r="I31" s="140"/>
       <c r="J31" s="140"/>
     </row>
-    <row r="32" spans="1:10" hidden="1">
+    <row r="32" spans="1:10">
       <c r="A32" s="156" t="s">
         <v>58</v>
       </c>
@@ -34135,7 +34122,7 @@
       <c r="I32" s="140"/>
       <c r="J32" s="140"/>
     </row>
-    <row r="33" spans="1:10" hidden="1">
+    <row r="33" spans="1:10">
       <c r="A33" s="156" t="s">
         <v>58</v>
       </c>
@@ -34161,7 +34148,7 @@
       <c r="I33" s="140"/>
       <c r="J33" s="140"/>
     </row>
-    <row r="34" spans="1:10" hidden="1">
+    <row r="34" spans="1:10">
       <c r="A34" s="156" t="s">
         <v>58</v>
       </c>
@@ -34189,7 +34176,7 @@
       <c r="I34" s="140"/>
       <c r="J34" s="140"/>
     </row>
-    <row r="35" spans="1:10" hidden="1">
+    <row r="35" spans="1:10">
       <c r="A35" s="156" t="s">
         <v>58</v>
       </c>
@@ -34217,7 +34204,7 @@
       <c r="I35" s="140"/>
       <c r="J35" s="140"/>
     </row>
-    <row r="36" spans="1:10" hidden="1">
+    <row r="36" spans="1:10">
       <c r="A36" s="156" t="s">
         <v>58</v>
       </c>
@@ -34243,7 +34230,7 @@
       <c r="I36" s="140"/>
       <c r="J36" s="140"/>
     </row>
-    <row r="37" spans="1:10" hidden="1">
+    <row r="37" spans="1:10">
       <c r="A37" s="156" t="s">
         <v>58</v>
       </c>
@@ -34269,7 +34256,7 @@
       <c r="I37" s="140"/>
       <c r="J37" s="140"/>
     </row>
-    <row r="38" spans="1:10" hidden="1">
+    <row r="38" spans="1:10">
       <c r="A38" s="156" t="s">
         <v>58</v>
       </c>
@@ -34295,7 +34282,7 @@
       <c r="I38" s="140"/>
       <c r="J38" s="140"/>
     </row>
-    <row r="39" spans="1:10" hidden="1">
+    <row r="39" spans="1:10">
       <c r="A39" s="156" t="s">
         <v>58</v>
       </c>
@@ -34321,7 +34308,7 @@
       <c r="I39" s="140"/>
       <c r="J39" s="140"/>
     </row>
-    <row r="40" spans="1:10" hidden="1">
+    <row r="40" spans="1:10">
       <c r="A40" s="156" t="s">
         <v>58</v>
       </c>
@@ -34347,7 +34334,7 @@
       <c r="I40" s="140"/>
       <c r="J40" s="140"/>
     </row>
-    <row r="41" spans="1:10" hidden="1">
+    <row r="41" spans="1:10">
       <c r="A41" s="156" t="s">
         <v>58</v>
       </c>
@@ -34373,7 +34360,7 @@
       <c r="I41" s="140"/>
       <c r="J41" s="140"/>
     </row>
-    <row r="42" spans="1:10" hidden="1">
+    <row r="42" spans="1:10">
       <c r="A42" s="156" t="s">
         <v>58</v>
       </c>
@@ -34401,7 +34388,7 @@
       <c r="I42" s="140"/>
       <c r="J42" s="140"/>
     </row>
-    <row r="43" spans="1:10" hidden="1">
+    <row r="43" spans="1:10">
       <c r="A43" s="156" t="s">
         <v>58</v>
       </c>
@@ -34429,7 +34416,7 @@
       <c r="I43" s="140"/>
       <c r="J43" s="140"/>
     </row>
-    <row r="44" spans="1:10" hidden="1">
+    <row r="44" spans="1:10">
       <c r="A44" s="156" t="s">
         <v>58</v>
       </c>
@@ -34457,7 +34444,7 @@
       <c r="I44" s="140"/>
       <c r="J44" s="140"/>
     </row>
-    <row r="45" spans="1:10" hidden="1">
+    <row r="45" spans="1:10">
       <c r="A45" s="156" t="s">
         <v>58</v>
       </c>
@@ -34485,7 +34472,7 @@
       <c r="I45" s="140"/>
       <c r="J45" s="140"/>
     </row>
-    <row r="46" spans="1:10" hidden="1">
+    <row r="46" spans="1:10">
       <c r="A46" s="156" t="s">
         <v>58</v>
       </c>
@@ -34513,7 +34500,7 @@
       <c r="I46" s="140"/>
       <c r="J46" s="140"/>
     </row>
-    <row r="47" spans="1:10" hidden="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="156" t="s">
         <v>58</v>
       </c>
@@ -34539,7 +34526,7 @@
       <c r="I47" s="140"/>
       <c r="J47" s="140"/>
     </row>
-    <row r="48" spans="1:10" hidden="1">
+    <row r="48" spans="1:10">
       <c r="A48" s="156" t="s">
         <v>58</v>
       </c>
@@ -36316,7 +36303,7 @@
       <c r="I113" s="140"/>
       <c r="J113" s="140"/>
     </row>
-    <row r="114" spans="1:10" hidden="1">
+    <row r="114" spans="1:10">
       <c r="D114" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36331,7 +36318,7 @@
       <c r="I114" s="140"/>
       <c r="J114" s="140"/>
     </row>
-    <row r="115" spans="1:10" hidden="1">
+    <row r="115" spans="1:10">
       <c r="D115" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36346,7 +36333,7 @@
       <c r="I115" s="140"/>
       <c r="J115" s="140"/>
     </row>
-    <row r="116" spans="1:10" hidden="1">
+    <row r="116" spans="1:10">
       <c r="D116" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36361,7 +36348,7 @@
       <c r="I116" s="140"/>
       <c r="J116" s="140"/>
     </row>
-    <row r="117" spans="1:10" hidden="1">
+    <row r="117" spans="1:10">
       <c r="D117" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36376,7 +36363,7 @@
       <c r="I117" s="140"/>
       <c r="J117" s="140"/>
     </row>
-    <row r="118" spans="1:10" hidden="1">
+    <row r="118" spans="1:10">
       <c r="D118" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36391,7 +36378,7 @@
       <c r="I118" s="140"/>
       <c r="J118" s="140"/>
     </row>
-    <row r="119" spans="1:10" hidden="1">
+    <row r="119" spans="1:10">
       <c r="D119" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36406,7 +36393,7 @@
       <c r="I119" s="140"/>
       <c r="J119" s="140"/>
     </row>
-    <row r="120" spans="1:10" hidden="1">
+    <row r="120" spans="1:10">
       <c r="D120" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36421,7 +36408,7 @@
       <c r="I120" s="140"/>
       <c r="J120" s="140"/>
     </row>
-    <row r="121" spans="1:10" hidden="1">
+    <row r="121" spans="1:10">
       <c r="D121" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36436,7 +36423,7 @@
       <c r="I121" s="140"/>
       <c r="J121" s="140"/>
     </row>
-    <row r="122" spans="1:10" hidden="1">
+    <row r="122" spans="1:10">
       <c r="D122" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36451,7 +36438,7 @@
       <c r="I122" s="140"/>
       <c r="J122" s="140"/>
     </row>
-    <row r="123" spans="1:10" hidden="1">
+    <row r="123" spans="1:10">
       <c r="D123" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36466,7 +36453,7 @@
       <c r="I123" s="140"/>
       <c r="J123" s="140"/>
     </row>
-    <row r="124" spans="1:10" hidden="1">
+    <row r="124" spans="1:10">
       <c r="D124" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36481,7 +36468,7 @@
       <c r="I124" s="140"/>
       <c r="J124" s="140"/>
     </row>
-    <row r="125" spans="1:10" hidden="1">
+    <row r="125" spans="1:10">
       <c r="D125" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36496,7 +36483,7 @@
       <c r="I125" s="140"/>
       <c r="J125" s="140"/>
     </row>
-    <row r="126" spans="1:10" hidden="1">
+    <row r="126" spans="1:10">
       <c r="D126" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36511,7 +36498,7 @@
       <c r="I126" s="140"/>
       <c r="J126" s="140"/>
     </row>
-    <row r="127" spans="1:10" hidden="1">
+    <row r="127" spans="1:10">
       <c r="D127" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36526,7 +36513,7 @@
       <c r="I127" s="140"/>
       <c r="J127" s="140"/>
     </row>
-    <row r="128" spans="1:10" hidden="1">
+    <row r="128" spans="1:10">
       <c r="D128" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36541,7 +36528,7 @@
       <c r="I128" s="140"/>
       <c r="J128" s="140"/>
     </row>
-    <row r="129" spans="4:10" hidden="1">
+    <row r="129" spans="4:10">
       <c r="D129" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36556,7 +36543,7 @@
       <c r="I129" s="140"/>
       <c r="J129" s="140"/>
     </row>
-    <row r="130" spans="4:10" hidden="1">
+    <row r="130" spans="4:10">
       <c r="D130" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36571,7 +36558,7 @@
       <c r="I130" s="140"/>
       <c r="J130" s="140"/>
     </row>
-    <row r="131" spans="4:10" hidden="1">
+    <row r="131" spans="4:10">
       <c r="D131" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36586,7 +36573,7 @@
       <c r="I131" s="140"/>
       <c r="J131" s="140"/>
     </row>
-    <row r="132" spans="4:10" hidden="1">
+    <row r="132" spans="4:10">
       <c r="D132" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36601,7 +36588,7 @@
       <c r="I132" s="140"/>
       <c r="J132" s="140"/>
     </row>
-    <row r="133" spans="4:10" hidden="1">
+    <row r="133" spans="4:10">
       <c r="D133" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36616,7 +36603,7 @@
       <c r="I133" s="140"/>
       <c r="J133" s="140"/>
     </row>
-    <row r="134" spans="4:10" hidden="1">
+    <row r="134" spans="4:10">
       <c r="D134" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36631,7 +36618,7 @@
       <c r="I134" s="140"/>
       <c r="J134" s="140"/>
     </row>
-    <row r="135" spans="4:10" hidden="1">
+    <row r="135" spans="4:10">
       <c r="D135" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36646,7 +36633,7 @@
       <c r="I135" s="140"/>
       <c r="J135" s="140"/>
     </row>
-    <row r="136" spans="4:10" hidden="1">
+    <row r="136" spans="4:10">
       <c r="D136" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36661,7 +36648,7 @@
       <c r="I136" s="140"/>
       <c r="J136" s="140"/>
     </row>
-    <row r="137" spans="4:10" hidden="1">
+    <row r="137" spans="4:10">
       <c r="D137" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36676,7 +36663,7 @@
       <c r="I137" s="140"/>
       <c r="J137" s="140"/>
     </row>
-    <row r="138" spans="4:10" hidden="1">
+    <row r="138" spans="4:10">
       <c r="D138" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36691,7 +36678,7 @@
       <c r="I138" s="140"/>
       <c r="J138" s="140"/>
     </row>
-    <row r="139" spans="4:10" hidden="1">
+    <row r="139" spans="4:10">
       <c r="D139" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36706,7 +36693,7 @@
       <c r="I139" s="140"/>
       <c r="J139" s="140"/>
     </row>
-    <row r="140" spans="4:10" hidden="1">
+    <row r="140" spans="4:10">
       <c r="D140" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36721,7 +36708,7 @@
       <c r="I140" s="140"/>
       <c r="J140" s="140"/>
     </row>
-    <row r="141" spans="4:10" hidden="1">
+    <row r="141" spans="4:10">
       <c r="D141" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36736,7 +36723,7 @@
       <c r="I141" s="140"/>
       <c r="J141" s="140"/>
     </row>
-    <row r="142" spans="4:10" hidden="1">
+    <row r="142" spans="4:10">
       <c r="D142" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -36751,7 +36738,7 @@
       <c r="I142" s="140"/>
       <c r="J142" s="140"/>
     </row>
-    <row r="143" spans="4:10" hidden="1">
+    <row r="143" spans="4:10">
       <c r="D143" s="79" t="e">
         <f t="shared" ref="D143:D174" si="10">E143*(1+$T$1)</f>
         <v>#DIV/0!</v>
@@ -36766,7 +36753,7 @@
       <c r="I143" s="140"/>
       <c r="J143" s="140"/>
     </row>
-    <row r="144" spans="4:10" hidden="1">
+    <row r="144" spans="4:10">
       <c r="D144" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36781,7 +36768,7 @@
       <c r="I144" s="140"/>
       <c r="J144" s="140"/>
     </row>
-    <row r="145" spans="4:10" hidden="1">
+    <row r="145" spans="4:10">
       <c r="D145" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36796,7 +36783,7 @@
       <c r="I145" s="140"/>
       <c r="J145" s="140"/>
     </row>
-    <row r="146" spans="4:10" hidden="1">
+    <row r="146" spans="4:10">
       <c r="D146" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36811,7 +36798,7 @@
       <c r="I146" s="140"/>
       <c r="J146" s="140"/>
     </row>
-    <row r="147" spans="4:10" hidden="1">
+    <row r="147" spans="4:10">
       <c r="D147" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36826,7 +36813,7 @@
       <c r="I147" s="140"/>
       <c r="J147" s="140"/>
     </row>
-    <row r="148" spans="4:10" hidden="1">
+    <row r="148" spans="4:10">
       <c r="D148" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36841,7 +36828,7 @@
       <c r="I148" s="140"/>
       <c r="J148" s="140"/>
     </row>
-    <row r="149" spans="4:10" hidden="1">
+    <row r="149" spans="4:10">
       <c r="D149" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36856,7 +36843,7 @@
       <c r="I149" s="140"/>
       <c r="J149" s="140"/>
     </row>
-    <row r="150" spans="4:10" hidden="1">
+    <row r="150" spans="4:10">
       <c r="D150" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36871,7 +36858,7 @@
       <c r="I150" s="140"/>
       <c r="J150" s="140"/>
     </row>
-    <row r="151" spans="4:10" hidden="1">
+    <row r="151" spans="4:10">
       <c r="D151" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36886,7 +36873,7 @@
       <c r="I151" s="140"/>
       <c r="J151" s="140"/>
     </row>
-    <row r="152" spans="4:10" hidden="1">
+    <row r="152" spans="4:10">
       <c r="D152" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36901,7 +36888,7 @@
       <c r="I152" s="140"/>
       <c r="J152" s="140"/>
     </row>
-    <row r="153" spans="4:10" hidden="1">
+    <row r="153" spans="4:10">
       <c r="D153" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36916,7 +36903,7 @@
       <c r="I153" s="140"/>
       <c r="J153" s="140"/>
     </row>
-    <row r="154" spans="4:10" hidden="1">
+    <row r="154" spans="4:10">
       <c r="D154" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36931,7 +36918,7 @@
       <c r="I154" s="140"/>
       <c r="J154" s="140"/>
     </row>
-    <row r="155" spans="4:10" hidden="1">
+    <row r="155" spans="4:10">
       <c r="D155" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36946,7 +36933,7 @@
       <c r="I155" s="140"/>
       <c r="J155" s="140"/>
     </row>
-    <row r="156" spans="4:10" hidden="1">
+    <row r="156" spans="4:10">
       <c r="D156" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36961,7 +36948,7 @@
       <c r="I156" s="140"/>
       <c r="J156" s="140"/>
     </row>
-    <row r="157" spans="4:10" hidden="1">
+    <row r="157" spans="4:10">
       <c r="D157" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36976,7 +36963,7 @@
       <c r="I157" s="140"/>
       <c r="J157" s="140"/>
     </row>
-    <row r="158" spans="4:10" hidden="1">
+    <row r="158" spans="4:10">
       <c r="D158" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -36991,7 +36978,7 @@
       <c r="I158" s="140"/>
       <c r="J158" s="140"/>
     </row>
-    <row r="159" spans="4:10" hidden="1">
+    <row r="159" spans="4:10">
       <c r="D159" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -37006,7 +36993,7 @@
       <c r="I159" s="140"/>
       <c r="J159" s="140"/>
     </row>
-    <row r="160" spans="4:10" hidden="1">
+    <row r="160" spans="4:10">
       <c r="D160" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -37021,7 +37008,7 @@
       <c r="I160" s="140"/>
       <c r="J160" s="140"/>
     </row>
-    <row r="161" spans="4:10" hidden="1">
+    <row r="161" spans="4:10">
       <c r="D161" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -37036,7 +37023,7 @@
       <c r="I161" s="140"/>
       <c r="J161" s="140"/>
     </row>
-    <row r="162" spans="4:10" hidden="1">
+    <row r="162" spans="4:10">
       <c r="D162" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -37051,7 +37038,7 @@
       <c r="I162" s="140"/>
       <c r="J162" s="140"/>
     </row>
-    <row r="163" spans="4:10" hidden="1">
+    <row r="163" spans="4:10">
       <c r="D163" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -37066,7 +37053,7 @@
       <c r="I163" s="140"/>
       <c r="J163" s="140"/>
     </row>
-    <row r="164" spans="4:10" hidden="1">
+    <row r="164" spans="4:10">
       <c r="D164" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -37081,7 +37068,7 @@
       <c r="I164" s="140"/>
       <c r="J164" s="140"/>
     </row>
-    <row r="165" spans="4:10" hidden="1">
+    <row r="165" spans="4:10">
       <c r="D165" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -37096,7 +37083,7 @@
       <c r="I165" s="140"/>
       <c r="J165" s="140"/>
     </row>
-    <row r="166" spans="4:10" hidden="1">
+    <row r="166" spans="4:10">
       <c r="D166" s="79" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
@@ -37111,7 +37098,7 @@
       <c r="I166" s="140"/>
       <c r="J166" s="140"/>
     </row>
-    <row r="167" spans="4:10" hidden="1">
+    <row r="167" spans="4:10">
       <c r="D167" s="79" t="e">
         <f t="shared" ref="D167:D198" si="12">E167*(1+$O$1)</f>
         <v>#DIV/0!</v>
@@ -37126,7 +37113,7 @@
       <c r="I167" s="140"/>
       <c r="J167" s="140"/>
     </row>
-    <row r="168" spans="4:10" hidden="1">
+    <row r="168" spans="4:10">
       <c r="D168" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37141,7 +37128,7 @@
       <c r="I168" s="140"/>
       <c r="J168" s="140"/>
     </row>
-    <row r="169" spans="4:10" hidden="1">
+    <row r="169" spans="4:10">
       <c r="D169" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37156,7 +37143,7 @@
       <c r="I169" s="140"/>
       <c r="J169" s="140"/>
     </row>
-    <row r="170" spans="4:10" hidden="1">
+    <row r="170" spans="4:10">
       <c r="D170" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37171,7 +37158,7 @@
       <c r="I170" s="140"/>
       <c r="J170" s="140"/>
     </row>
-    <row r="171" spans="4:10" hidden="1">
+    <row r="171" spans="4:10">
       <c r="D171" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37186,7 +37173,7 @@
       <c r="I171" s="140"/>
       <c r="J171" s="140"/>
     </row>
-    <row r="172" spans="4:10" hidden="1">
+    <row r="172" spans="4:10">
       <c r="D172" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37201,7 +37188,7 @@
       <c r="I172" s="140"/>
       <c r="J172" s="140"/>
     </row>
-    <row r="173" spans="4:10" hidden="1">
+    <row r="173" spans="4:10">
       <c r="D173" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37216,7 +37203,7 @@
       <c r="I173" s="140"/>
       <c r="J173" s="140"/>
     </row>
-    <row r="174" spans="4:10" hidden="1">
+    <row r="174" spans="4:10">
       <c r="D174" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37231,7 +37218,7 @@
       <c r="I174" s="140"/>
       <c r="J174" s="140"/>
     </row>
-    <row r="175" spans="4:10" hidden="1">
+    <row r="175" spans="4:10">
       <c r="D175" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37246,7 +37233,7 @@
       <c r="I175" s="140"/>
       <c r="J175" s="140"/>
     </row>
-    <row r="176" spans="4:10" hidden="1">
+    <row r="176" spans="4:10">
       <c r="D176" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37261,7 +37248,7 @@
       <c r="I176" s="140"/>
       <c r="J176" s="140"/>
     </row>
-    <row r="177" spans="4:10" hidden="1">
+    <row r="177" spans="4:10">
       <c r="D177" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37276,7 +37263,7 @@
       <c r="I177" s="140"/>
       <c r="J177" s="140"/>
     </row>
-    <row r="178" spans="4:10" hidden="1">
+    <row r="178" spans="4:10">
       <c r="D178" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37291,7 +37278,7 @@
       <c r="I178" s="140"/>
       <c r="J178" s="140"/>
     </row>
-    <row r="179" spans="4:10" hidden="1">
+    <row r="179" spans="4:10">
       <c r="D179" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37306,7 +37293,7 @@
       <c r="I179" s="140"/>
       <c r="J179" s="140"/>
     </row>
-    <row r="180" spans="4:10" hidden="1">
+    <row r="180" spans="4:10">
       <c r="D180" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37321,7 +37308,7 @@
       <c r="I180" s="140"/>
       <c r="J180" s="140"/>
     </row>
-    <row r="181" spans="4:10" hidden="1">
+    <row r="181" spans="4:10">
       <c r="D181" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37336,7 +37323,7 @@
       <c r="I181" s="140"/>
       <c r="J181" s="140"/>
     </row>
-    <row r="182" spans="4:10" hidden="1">
+    <row r="182" spans="4:10">
       <c r="D182" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37351,7 +37338,7 @@
       <c r="I182" s="140"/>
       <c r="J182" s="140"/>
     </row>
-    <row r="183" spans="4:10" hidden="1">
+    <row r="183" spans="4:10">
       <c r="D183" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37366,7 +37353,7 @@
       <c r="I183" s="140"/>
       <c r="J183" s="140"/>
     </row>
-    <row r="184" spans="4:10" hidden="1">
+    <row r="184" spans="4:10">
       <c r="D184" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37381,7 +37368,7 @@
       <c r="I184" s="140"/>
       <c r="J184" s="140"/>
     </row>
-    <row r="185" spans="4:10" hidden="1">
+    <row r="185" spans="4:10">
       <c r="D185" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37396,7 +37383,7 @@
       <c r="I185" s="140"/>
       <c r="J185" s="140"/>
     </row>
-    <row r="186" spans="4:10" hidden="1">
+    <row r="186" spans="4:10">
       <c r="D186" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37411,7 +37398,7 @@
       <c r="I186" s="140"/>
       <c r="J186" s="140"/>
     </row>
-    <row r="187" spans="4:10" hidden="1">
+    <row r="187" spans="4:10">
       <c r="D187" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37426,7 +37413,7 @@
       <c r="I187" s="140"/>
       <c r="J187" s="140"/>
     </row>
-    <row r="188" spans="4:10" hidden="1">
+    <row r="188" spans="4:10">
       <c r="D188" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37441,7 +37428,7 @@
       <c r="I188" s="140"/>
       <c r="J188" s="140"/>
     </row>
-    <row r="189" spans="4:10" hidden="1">
+    <row r="189" spans="4:10">
       <c r="D189" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37456,7 +37443,7 @@
       <c r="I189" s="140"/>
       <c r="J189" s="140"/>
     </row>
-    <row r="190" spans="4:10" hidden="1">
+    <row r="190" spans="4:10">
       <c r="D190" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37471,7 +37458,7 @@
       <c r="I190" s="140"/>
       <c r="J190" s="140"/>
     </row>
-    <row r="191" spans="4:10" hidden="1">
+    <row r="191" spans="4:10">
       <c r="D191" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37486,7 +37473,7 @@
       <c r="I191" s="140"/>
       <c r="J191" s="140"/>
     </row>
-    <row r="192" spans="4:10" hidden="1">
+    <row r="192" spans="4:10">
       <c r="D192" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37501,7 +37488,7 @@
       <c r="I192" s="140"/>
       <c r="J192" s="140"/>
     </row>
-    <row r="193" spans="4:10" hidden="1">
+    <row r="193" spans="4:10">
       <c r="D193" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37516,7 +37503,7 @@
       <c r="I193" s="140"/>
       <c r="J193" s="140"/>
     </row>
-    <row r="194" spans="4:10" hidden="1">
+    <row r="194" spans="4:10">
       <c r="D194" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37531,7 +37518,7 @@
       <c r="I194" s="140"/>
       <c r="J194" s="140"/>
     </row>
-    <row r="195" spans="4:10" hidden="1">
+    <row r="195" spans="4:10">
       <c r="D195" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37546,7 +37533,7 @@
       <c r="I195" s="140"/>
       <c r="J195" s="140"/>
     </row>
-    <row r="196" spans="4:10" hidden="1">
+    <row r="196" spans="4:10">
       <c r="D196" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37561,7 +37548,7 @@
       <c r="I196" s="140"/>
       <c r="J196" s="140"/>
     </row>
-    <row r="197" spans="4:10" hidden="1">
+    <row r="197" spans="4:10">
       <c r="D197" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37576,7 +37563,7 @@
       <c r="I197" s="140"/>
       <c r="J197" s="140"/>
     </row>
-    <row r="198" spans="4:10" hidden="1">
+    <row r="198" spans="4:10">
       <c r="D198" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -37591,7 +37578,7 @@
       <c r="I198" s="140"/>
       <c r="J198" s="140"/>
     </row>
-    <row r="199" spans="4:10" hidden="1">
+    <row r="199" spans="4:10">
       <c r="D199" s="79" t="e">
         <f t="shared" ref="D199:D230" si="14">E199*(1+$O$1)</f>
         <v>#DIV/0!</v>
@@ -37606,7 +37593,7 @@
       <c r="I199" s="140"/>
       <c r="J199" s="140"/>
     </row>
-    <row r="200" spans="4:10" hidden="1">
+    <row r="200" spans="4:10">
       <c r="D200" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37621,7 +37608,7 @@
       <c r="I200" s="140"/>
       <c r="J200" s="140"/>
     </row>
-    <row r="201" spans="4:10" hidden="1">
+    <row r="201" spans="4:10">
       <c r="D201" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37636,7 +37623,7 @@
       <c r="I201" s="140"/>
       <c r="J201" s="140"/>
     </row>
-    <row r="202" spans="4:10" hidden="1">
+    <row r="202" spans="4:10">
       <c r="D202" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37651,7 +37638,7 @@
       <c r="I202" s="140"/>
       <c r="J202" s="140"/>
     </row>
-    <row r="203" spans="4:10" hidden="1">
+    <row r="203" spans="4:10">
       <c r="D203" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37666,7 +37653,7 @@
       <c r="I203" s="140"/>
       <c r="J203" s="140"/>
     </row>
-    <row r="204" spans="4:10" hidden="1">
+    <row r="204" spans="4:10">
       <c r="D204" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37681,7 +37668,7 @@
       <c r="I204" s="140"/>
       <c r="J204" s="140"/>
     </row>
-    <row r="205" spans="4:10" hidden="1">
+    <row r="205" spans="4:10">
       <c r="D205" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37696,7 +37683,7 @@
       <c r="I205" s="140"/>
       <c r="J205" s="140"/>
     </row>
-    <row r="206" spans="4:10" hidden="1">
+    <row r="206" spans="4:10">
       <c r="D206" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37711,7 +37698,7 @@
       <c r="I206" s="140"/>
       <c r="J206" s="140"/>
     </row>
-    <row r="207" spans="4:10" hidden="1">
+    <row r="207" spans="4:10">
       <c r="D207" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37726,7 +37713,7 @@
       <c r="I207" s="140"/>
       <c r="J207" s="140"/>
     </row>
-    <row r="208" spans="4:10" hidden="1">
+    <row r="208" spans="4:10">
       <c r="D208" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37741,7 +37728,7 @@
       <c r="I208" s="140"/>
       <c r="J208" s="140"/>
     </row>
-    <row r="209" spans="4:10" hidden="1">
+    <row r="209" spans="4:10">
       <c r="D209" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37756,7 +37743,7 @@
       <c r="I209" s="140"/>
       <c r="J209" s="140"/>
     </row>
-    <row r="210" spans="4:10" hidden="1">
+    <row r="210" spans="4:10">
       <c r="D210" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37771,7 +37758,7 @@
       <c r="I210" s="140"/>
       <c r="J210" s="140"/>
     </row>
-    <row r="211" spans="4:10" hidden="1">
+    <row r="211" spans="4:10">
       <c r="D211" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37786,7 +37773,7 @@
       <c r="I211" s="140"/>
       <c r="J211" s="140"/>
     </row>
-    <row r="212" spans="4:10" hidden="1">
+    <row r="212" spans="4:10">
       <c r="D212" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37801,7 +37788,7 @@
       <c r="I212" s="140"/>
       <c r="J212" s="140"/>
     </row>
-    <row r="213" spans="4:10" hidden="1">
+    <row r="213" spans="4:10">
       <c r="D213" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37816,7 +37803,7 @@
       <c r="I213" s="140"/>
       <c r="J213" s="140"/>
     </row>
-    <row r="214" spans="4:10" hidden="1">
+    <row r="214" spans="4:10">
       <c r="D214" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37831,7 +37818,7 @@
       <c r="I214" s="140"/>
       <c r="J214" s="140"/>
     </row>
-    <row r="215" spans="4:10" hidden="1">
+    <row r="215" spans="4:10">
       <c r="D215" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37846,7 +37833,7 @@
       <c r="I215" s="140"/>
       <c r="J215" s="140"/>
     </row>
-    <row r="216" spans="4:10" hidden="1">
+    <row r="216" spans="4:10">
       <c r="D216" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37861,7 +37848,7 @@
       <c r="I216" s="140"/>
       <c r="J216" s="140"/>
     </row>
-    <row r="217" spans="4:10" hidden="1">
+    <row r="217" spans="4:10">
       <c r="D217" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37876,7 +37863,7 @@
       <c r="I217" s="140"/>
       <c r="J217" s="140"/>
     </row>
-    <row r="218" spans="4:10" hidden="1">
+    <row r="218" spans="4:10">
       <c r="D218" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37891,7 +37878,7 @@
       <c r="I218" s="140"/>
       <c r="J218" s="140"/>
     </row>
-    <row r="219" spans="4:10" hidden="1">
+    <row r="219" spans="4:10">
       <c r="D219" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37906,7 +37893,7 @@
       <c r="I219" s="140"/>
       <c r="J219" s="140"/>
     </row>
-    <row r="220" spans="4:10" hidden="1">
+    <row r="220" spans="4:10">
       <c r="D220" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37921,7 +37908,7 @@
       <c r="I220" s="140"/>
       <c r="J220" s="140"/>
     </row>
-    <row r="221" spans="4:10" hidden="1">
+    <row r="221" spans="4:10">
       <c r="D221" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37936,7 +37923,7 @@
       <c r="I221" s="140"/>
       <c r="J221" s="140"/>
     </row>
-    <row r="222" spans="4:10" hidden="1">
+    <row r="222" spans="4:10">
       <c r="D222" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37951,7 +37938,7 @@
       <c r="I222" s="140"/>
       <c r="J222" s="140"/>
     </row>
-    <row r="223" spans="4:10" hidden="1">
+    <row r="223" spans="4:10">
       <c r="D223" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37966,7 +37953,7 @@
       <c r="I223" s="140"/>
       <c r="J223" s="140"/>
     </row>
-    <row r="224" spans="4:10" hidden="1">
+    <row r="224" spans="4:10">
       <c r="D224" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37981,7 +37968,7 @@
       <c r="I224" s="140"/>
       <c r="J224" s="140"/>
     </row>
-    <row r="225" spans="4:10" hidden="1">
+    <row r="225" spans="4:10">
       <c r="D225" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -37996,7 +37983,7 @@
       <c r="I225" s="140"/>
       <c r="J225" s="140"/>
     </row>
-    <row r="226" spans="4:10" hidden="1">
+    <row r="226" spans="4:10">
       <c r="D226" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -38011,7 +37998,7 @@
       <c r="I226" s="140"/>
       <c r="J226" s="140"/>
     </row>
-    <row r="227" spans="4:10" hidden="1">
+    <row r="227" spans="4:10">
       <c r="D227" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -38026,7 +38013,7 @@
       <c r="I227" s="140"/>
       <c r="J227" s="140"/>
     </row>
-    <row r="228" spans="4:10" hidden="1">
+    <row r="228" spans="4:10">
       <c r="D228" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -38041,7 +38028,7 @@
       <c r="I228" s="140"/>
       <c r="J228" s="140"/>
     </row>
-    <row r="229" spans="4:10" hidden="1">
+    <row r="229" spans="4:10">
       <c r="D229" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -38056,7 +38043,7 @@
       <c r="I229" s="140"/>
       <c r="J229" s="140"/>
     </row>
-    <row r="230" spans="4:10" hidden="1">
+    <row r="230" spans="4:10">
       <c r="D230" s="79" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
@@ -38071,7 +38058,7 @@
       <c r="I230" s="140"/>
       <c r="J230" s="140"/>
     </row>
-    <row r="231" spans="4:10" hidden="1">
+    <row r="231" spans="4:10">
       <c r="D231" s="79" t="e">
         <f t="shared" ref="D231:D262" si="16">E231*(1+$O$1)</f>
         <v>#DIV/0!</v>
@@ -38086,7 +38073,7 @@
       <c r="I231" s="140"/>
       <c r="J231" s="140"/>
     </row>
-    <row r="232" spans="4:10" hidden="1">
+    <row r="232" spans="4:10">
       <c r="D232" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38101,7 +38088,7 @@
       <c r="I232" s="140"/>
       <c r="J232" s="140"/>
     </row>
-    <row r="233" spans="4:10" hidden="1">
+    <row r="233" spans="4:10">
       <c r="D233" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38116,7 +38103,7 @@
       <c r="I233" s="140"/>
       <c r="J233" s="140"/>
     </row>
-    <row r="234" spans="4:10" hidden="1">
+    <row r="234" spans="4:10">
       <c r="D234" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38131,7 +38118,7 @@
       <c r="I234" s="140"/>
       <c r="J234" s="140"/>
     </row>
-    <row r="235" spans="4:10" hidden="1">
+    <row r="235" spans="4:10">
       <c r="D235" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38146,7 +38133,7 @@
       <c r="I235" s="140"/>
       <c r="J235" s="140"/>
     </row>
-    <row r="236" spans="4:10" hidden="1">
+    <row r="236" spans="4:10">
       <c r="D236" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38161,7 +38148,7 @@
       <c r="I236" s="140"/>
       <c r="J236" s="140"/>
     </row>
-    <row r="237" spans="4:10" hidden="1">
+    <row r="237" spans="4:10">
       <c r="D237" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38176,7 +38163,7 @@
       <c r="I237" s="140"/>
       <c r="J237" s="140"/>
     </row>
-    <row r="238" spans="4:10" hidden="1">
+    <row r="238" spans="4:10">
       <c r="D238" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38191,7 +38178,7 @@
       <c r="I238" s="140"/>
       <c r="J238" s="140"/>
     </row>
-    <row r="239" spans="4:10" hidden="1">
+    <row r="239" spans="4:10">
       <c r="D239" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38206,7 +38193,7 @@
       <c r="I239" s="140"/>
       <c r="J239" s="140"/>
     </row>
-    <row r="240" spans="4:10" hidden="1">
+    <row r="240" spans="4:10">
       <c r="D240" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38221,7 +38208,7 @@
       <c r="I240" s="140"/>
       <c r="J240" s="140"/>
     </row>
-    <row r="241" spans="1:10" hidden="1">
+    <row r="241" spans="1:10">
       <c r="D241" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38236,7 +38223,7 @@
       <c r="I241" s="140"/>
       <c r="J241" s="140"/>
     </row>
-    <row r="242" spans="1:10" hidden="1">
+    <row r="242" spans="1:10">
       <c r="D242" s="79" t="e">
         <f t="shared" si="16"/>
         <v>#DIV/0!</v>
@@ -38277,7 +38264,7 @@
       <c r="I243" s="140"/>
       <c r="J243" s="140"/>
     </row>
-    <row r="244" spans="1:10" hidden="1">
+    <row r="244" spans="1:10">
       <c r="A244" s="156" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
trying to add message saying "bouquet optimization underway; please be patient"
</commit_message>
<xml_diff>
--- a/data/CANONICAL Bouquet Recipe Master Sheet.xlsx
+++ b/data/CANONICAL Bouquet Recipe Master Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Documents/Sweet Piedmont/Offerings/Software and Code/bouquet-blueprint-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5182C39-71AB-1E42-B095-BB8790072E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7302CB7-6786-634A-A41C-CDF1B8CD2607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5060" yWindow="760" windowWidth="29500" windowHeight="21580" firstSheet="1" activeTab="1" xr2:uid="{835A2F5B-2282-E345-9D43-16C3FBECA701}"/>
   </bookViews>
@@ -33241,7 +33241,7 @@
   <dimension ref="A1:T246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C249" sqref="C249"/>
+      <selection activeCell="C255" sqref="C255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
not sure wtf is going on
</commit_message>
<xml_diff>
--- a/data/CANONICAL Bouquet Recipe Master Sheet.xlsx
+++ b/data/CANONICAL Bouquet Recipe Master Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Documents/Sweet Piedmont/Offerings/Software and Code/bouquet-blueprint-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083433DE-08A7-0845-ACCA-1BA8DE43E151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECA0657-F591-2A4E-A033-3D776C117237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5060" yWindow="760" windowWidth="29500" windowHeight="21580" firstSheet="1" activeTab="1" xr2:uid="{835A2F5B-2282-E345-9D43-16C3FBECA701}"/>
+    <workbookView xWindow="3640" yWindow="760" windowWidth="29500" windowHeight="21580" firstSheet="1" activeTab="1" xr2:uid="{835A2F5B-2282-E345-9D43-16C3FBECA701}"/>
   </bookViews>
   <sheets>
     <sheet name="IMPT INFO" sheetId="30" r:id="rId1"/>
@@ -520,7 +520,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId27"/>
+    <pivotCache cacheId="3" r:id="rId27"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4382,12 +4382,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4409,10 +4403,13 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4421,14 +4418,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4436,14 +4436,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4464,9 +4467,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -10043,7 +10043,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B2658901-0CBE-9C4B-BFF5-CAD078317D01}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B2658901-0CBE-9C4B-BFF5-CAD078317D01}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -10312,7 +10312,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B78D5962-5DD2-2E45-9817-5CEF79A2470C}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B78D5962-5DD2-2E45-9817-5CEF79A2470C}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -10703,7 +10703,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B7AE58DE-C14F-5241-BCB3-1D6E88366DE3}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B7AE58DE-C14F-5241-BCB3-1D6E88366DE3}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A73" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -11109,7 +11109,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85A6AB1C-7E0E-B54F-8BC1-2661D91D27AD}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85A6AB1C-7E0E-B54F-8BC1-2661D91D27AD}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A66" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -11495,7 +11495,16 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{63FB889B-362F-FA4D-9D4D-A49BD91E0CC2}" name="Table31615" displayName="Table31615" ref="A1:J246" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141" tableBorderDxfId="140" headerRowCellStyle="Currency" dataCellStyle="Currency">
-  <autoFilter ref="A1:J246" xr:uid="{63FB889B-362F-FA4D-9D4D-A49BD91E0CC2}"/>
+  <autoFilter ref="A1:J246" xr:uid="{63FB889B-362F-FA4D-9D4D-A49BD91E0CC2}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Early Spring"/>
+        <filter val="Early Spring, Late Spring"/>
+        <filter val="Early Spring, Late Spring, Summer/Fall"/>
+        <filter val="Early Spring, Summer/Fall"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J246">
     <sortCondition ref="B1:B246"/>
   </sortState>
@@ -30090,16 +30099,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33233,8 +33242,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="106" workbookViewId="0">
+      <selection activeCell="E252" sqref="E252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -33383,7 +33392,7 @@
       <c r="I4" s="140"/>
       <c r="J4" s="140"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" hidden="1">
       <c r="A5" t="s">
         <v>895</v>
       </c>
@@ -33409,7 +33418,7 @@
       <c r="I5" s="140"/>
       <c r="J5" s="140"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" hidden="1">
       <c r="A6" t="s">
         <v>145</v>
       </c>
@@ -33435,7 +33444,7 @@
       <c r="I6" s="140"/>
       <c r="J6" s="140"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" hidden="1">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -33461,7 +33470,7 @@
       <c r="I7" s="140"/>
       <c r="J7" s="140"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" hidden="1">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -33487,7 +33496,7 @@
       <c r="I8" s="140"/>
       <c r="J8" s="140"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" hidden="1">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -33515,7 +33524,7 @@
       <c r="I9" s="140"/>
       <c r="J9" s="140"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" hidden="1">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -33543,7 +33552,7 @@
       <c r="I10" s="140"/>
       <c r="J10" s="140"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" hidden="1">
       <c r="A11" s="156" t="s">
         <v>57</v>
       </c>
@@ -33571,7 +33580,7 @@
       <c r="I11" s="140"/>
       <c r="J11" s="140"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" hidden="1">
       <c r="A12" s="156" t="s">
         <v>57</v>
       </c>
@@ -33599,7 +33608,7 @@
       <c r="I12" s="140"/>
       <c r="J12" s="140"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" hidden="1">
       <c r="A13" s="156" t="s">
         <v>57</v>
       </c>
@@ -33761,7 +33770,7 @@
       <c r="I18" s="140"/>
       <c r="J18" s="140"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" hidden="1">
       <c r="A19" s="156" t="s">
         <v>57</v>
       </c>
@@ -33789,7 +33798,7 @@
       <c r="I19" s="140"/>
       <c r="J19" s="140"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" hidden="1">
       <c r="A20" s="156" t="s">
         <v>57</v>
       </c>
@@ -33817,7 +33826,7 @@
       <c r="I20" s="140"/>
       <c r="J20" s="140"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" hidden="1">
       <c r="A21" s="156" t="s">
         <v>57</v>
       </c>
@@ -33843,7 +33852,7 @@
       <c r="I21" s="140"/>
       <c r="J21" s="140"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22" s="156" t="s">
         <v>895</v>
       </c>
@@ -33869,7 +33878,7 @@
       <c r="I22" s="140"/>
       <c r="J22" s="140"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" hidden="1">
       <c r="A23" s="156" t="s">
         <v>895</v>
       </c>
@@ -33897,7 +33906,7 @@
       <c r="I23" s="140"/>
       <c r="J23" s="140"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" hidden="1">
       <c r="A24" s="156" t="s">
         <v>895</v>
       </c>
@@ -33923,7 +33932,7 @@
       <c r="I24" s="140"/>
       <c r="J24" s="140"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25" s="156" t="s">
         <v>895</v>
       </c>
@@ -33951,7 +33960,7 @@
       <c r="I25" s="140"/>
       <c r="J25" s="140"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" hidden="1">
       <c r="A26" s="156" t="s">
         <v>895</v>
       </c>
@@ -33977,7 +33986,7 @@
       <c r="I26" s="140"/>
       <c r="J26" s="140"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" hidden="1">
       <c r="A27" s="156" t="s">
         <v>145</v>
       </c>
@@ -34007,7 +34016,7 @@
       <c r="I27" s="140"/>
       <c r="J27" s="140"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" hidden="1">
       <c r="A28" s="156" t="s">
         <v>145</v>
       </c>
@@ -34033,7 +34042,7 @@
       <c r="I28" s="140"/>
       <c r="J28" s="140"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" hidden="1">
       <c r="A29" s="156" t="s">
         <v>145</v>
       </c>
@@ -34059,7 +34068,7 @@
       <c r="I29" s="140"/>
       <c r="J29" s="140"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" hidden="1">
       <c r="A30" s="156" t="s">
         <v>145</v>
       </c>
@@ -34085,7 +34094,7 @@
       <c r="I30" s="140"/>
       <c r="J30" s="140"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" hidden="1">
       <c r="A31" s="156" t="s">
         <v>145</v>
       </c>
@@ -34116,7 +34125,7 @@
       <c r="I31" s="140"/>
       <c r="J31" s="140"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" hidden="1">
       <c r="A32" s="156" t="s">
         <v>145</v>
       </c>
@@ -34142,7 +34151,7 @@
       <c r="I32" s="140"/>
       <c r="J32" s="140"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" hidden="1">
       <c r="A33" s="156" t="s">
         <v>145</v>
       </c>
@@ -34168,7 +34177,7 @@
       <c r="I33" s="140"/>
       <c r="J33" s="140"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" hidden="1">
       <c r="A34" s="156" t="s">
         <v>145</v>
       </c>
@@ -34179,7 +34188,7 @@
         <v>90</v>
       </c>
       <c r="D34" s="79">
-        <f t="shared" ref="D34:D65" si="2">E34*(1+$T$1)</f>
+        <f t="shared" ref="D34:D62" si="2">E34*(1+$T$1)</f>
         <v>2.0999999999999996</v>
       </c>
       <c r="E34" s="79">
@@ -34194,7 +34203,7 @@
       <c r="I34" s="140"/>
       <c r="J34" s="140"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" hidden="1">
       <c r="A35" s="156" t="s">
         <v>145</v>
       </c>
@@ -34220,7 +34229,7 @@
       <c r="I35" s="140"/>
       <c r="J35" s="140"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" hidden="1">
       <c r="A36" s="156" t="s">
         <v>145</v>
       </c>
@@ -34246,7 +34255,7 @@
       <c r="I36" s="140"/>
       <c r="J36" s="140"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" hidden="1">
       <c r="A37" s="156" t="s">
         <v>145</v>
       </c>
@@ -34274,7 +34283,7 @@
       <c r="I37" s="140"/>
       <c r="J37" s="140"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" hidden="1">
       <c r="A38" s="156" t="s">
         <v>895</v>
       </c>
@@ -34302,7 +34311,7 @@
       <c r="I38" s="140"/>
       <c r="J38" s="140"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" hidden="1">
       <c r="A39" s="156" t="s">
         <v>895</v>
       </c>
@@ -34488,7 +34497,7 @@
       <c r="I45" s="140"/>
       <c r="J45" s="140"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" hidden="1">
       <c r="A46" s="156" t="s">
         <v>57</v>
       </c>
@@ -34514,7 +34523,7 @@
       <c r="I46" s="140"/>
       <c r="J46" s="140"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" hidden="1">
       <c r="A47" s="156" t="s">
         <v>57</v>
       </c>
@@ -34540,7 +34549,7 @@
       <c r="I47" s="140"/>
       <c r="J47" s="140"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" hidden="1">
       <c r="A48" s="156" t="s">
         <v>57</v>
       </c>
@@ -34566,7 +34575,7 @@
       <c r="I48" s="140"/>
       <c r="J48" s="140"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" hidden="1">
       <c r="A49" s="156" t="s">
         <v>57</v>
       </c>
@@ -34618,7 +34627,7 @@
       <c r="I50" s="140"/>
       <c r="J50" s="140"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" hidden="1">
       <c r="A51" s="156" t="s">
         <v>895</v>
       </c>
@@ -34644,7 +34653,7 @@
       <c r="I51" s="140"/>
       <c r="J51" s="140"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" hidden="1">
       <c r="A52" s="156" t="s">
         <v>895</v>
       </c>
@@ -34670,7 +34679,7 @@
       <c r="I52" s="140"/>
       <c r="J52" s="140"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" hidden="1">
       <c r="A53" s="156" t="s">
         <v>895</v>
       </c>
@@ -34698,7 +34707,7 @@
       <c r="I53" s="140"/>
       <c r="J53" s="140"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" hidden="1">
       <c r="A54" s="156" t="s">
         <v>145</v>
       </c>
@@ -34728,7 +34737,7 @@
       <c r="I54" s="140"/>
       <c r="J54" s="140"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" hidden="1">
       <c r="A55" s="156" t="s">
         <v>145</v>
       </c>
@@ -34754,7 +34763,7 @@
       <c r="I55" s="140"/>
       <c r="J55" s="140"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" hidden="1">
       <c r="A56" s="156" t="s">
         <v>145</v>
       </c>
@@ -34784,7 +34793,7 @@
       <c r="I56" s="140"/>
       <c r="J56" s="140"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" hidden="1">
       <c r="A57" s="156" t="s">
         <v>145</v>
       </c>
@@ -34810,7 +34819,7 @@
       <c r="I57" s="140"/>
       <c r="J57" s="140"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" hidden="1">
       <c r="A58" s="156" t="s">
         <v>145</v>
       </c>
@@ -34836,7 +34845,7 @@
       <c r="I58" s="140"/>
       <c r="J58" s="140"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" hidden="1">
       <c r="A59" s="156" t="s">
         <v>895</v>
       </c>
@@ -34864,7 +34873,7 @@
       <c r="I59" s="140"/>
       <c r="J59" s="140"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" hidden="1">
       <c r="A60" s="156" t="s">
         <v>895</v>
       </c>
@@ -34892,7 +34901,7 @@
       <c r="I60" s="140"/>
       <c r="J60" s="140"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" hidden="1">
       <c r="A61" s="156" t="s">
         <v>145</v>
       </c>
@@ -34918,7 +34927,7 @@
       <c r="I61" s="140"/>
       <c r="J61" s="140"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" hidden="1">
       <c r="A62" s="156" t="s">
         <v>57</v>
       </c>
@@ -35076,7 +35085,7 @@
       <c r="I67" s="140"/>
       <c r="J67" s="140"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" hidden="1">
       <c r="A68" s="156" t="s">
         <v>57</v>
       </c>
@@ -35102,7 +35111,7 @@
       <c r="I68" s="140"/>
       <c r="J68" s="140"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" hidden="1">
       <c r="A69" s="156" t="s">
         <v>895</v>
       </c>
@@ -35128,7 +35137,7 @@
       <c r="I69" s="140"/>
       <c r="J69" s="140"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" hidden="1">
       <c r="A70" s="156" t="s">
         <v>895</v>
       </c>
@@ -35156,7 +35165,7 @@
       <c r="I70" s="140"/>
       <c r="J70" s="140"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" hidden="1">
       <c r="A71" s="156" t="s">
         <v>145</v>
       </c>
@@ -35182,7 +35191,7 @@
       <c r="I71" s="140"/>
       <c r="J71" s="140"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" hidden="1">
       <c r="A72" s="156" t="s">
         <v>145</v>
       </c>
@@ -35208,7 +35217,7 @@
       <c r="I72" s="140"/>
       <c r="J72" s="140"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" hidden="1">
       <c r="A73" s="156" t="s">
         <v>145</v>
       </c>
@@ -35234,7 +35243,7 @@
       <c r="I73" s="140"/>
       <c r="J73" s="140"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" hidden="1">
       <c r="A74" s="156" t="s">
         <v>145</v>
       </c>
@@ -35262,7 +35271,7 @@
       <c r="I74" s="140"/>
       <c r="J74" s="140"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" hidden="1">
       <c r="A75" s="156" t="s">
         <v>145</v>
       </c>
@@ -35288,7 +35297,7 @@
       <c r="I75" s="140"/>
       <c r="J75" s="140"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" hidden="1">
       <c r="A76" s="156" t="s">
         <v>145</v>
       </c>
@@ -35316,7 +35325,7 @@
       <c r="I76" s="140"/>
       <c r="J76" s="140"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" hidden="1">
       <c r="A77" s="156" t="s">
         <v>145</v>
       </c>
@@ -35342,7 +35351,7 @@
       <c r="I77" s="140"/>
       <c r="J77" s="140"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" hidden="1">
       <c r="A78" s="156" t="s">
         <v>145</v>
       </c>
@@ -35368,7 +35377,7 @@
       <c r="I78" s="140"/>
       <c r="J78" s="140"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" hidden="1">
       <c r="A79" s="156" t="s">
         <v>145</v>
       </c>
@@ -35394,7 +35403,7 @@
       <c r="I79" s="140"/>
       <c r="J79" s="140"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" hidden="1">
       <c r="A80" s="156" t="s">
         <v>895</v>
       </c>
@@ -35424,7 +35433,7 @@
       <c r="I80" s="140"/>
       <c r="J80" s="140"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" hidden="1">
       <c r="A81" s="156" t="s">
         <v>895</v>
       </c>
@@ -35480,7 +35489,7 @@
       <c r="I82" s="140"/>
       <c r="J82" s="140"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" hidden="1">
       <c r="A83" s="156" t="s">
         <v>57</v>
       </c>
@@ -35506,7 +35515,7 @@
       <c r="I83" s="140"/>
       <c r="J83" s="140"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" hidden="1">
       <c r="A84" s="156" t="s">
         <v>57</v>
       </c>
@@ -35532,7 +35541,7 @@
       <c r="I84" s="140"/>
       <c r="J84" s="140"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" hidden="1">
       <c r="A85" s="94" t="s">
         <v>57</v>
       </c>
@@ -35558,7 +35567,7 @@
       <c r="I85" s="140"/>
       <c r="J85" s="140"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" hidden="1">
       <c r="A86" s="96" t="s">
         <v>57</v>
       </c>
@@ -35586,7 +35595,7 @@
       <c r="I86" s="140"/>
       <c r="J86" s="140"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" hidden="1">
       <c r="A87" t="s">
         <v>57</v>
       </c>
@@ -35614,7 +35623,7 @@
       <c r="I87" s="140"/>
       <c r="J87" s="140"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" hidden="1">
       <c r="A88" t="s">
         <v>57</v>
       </c>
@@ -35640,7 +35649,7 @@
       <c r="I88" s="140"/>
       <c r="J88" s="140"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" hidden="1">
       <c r="A89" t="s">
         <v>57</v>
       </c>
@@ -35722,7 +35731,7 @@
       <c r="I91" s="140"/>
       <c r="J91" s="140"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" hidden="1">
       <c r="A92" t="s">
         <v>895</v>
       </c>
@@ -35750,7 +35759,7 @@
       <c r="I92" s="140"/>
       <c r="J92" s="140"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" hidden="1">
       <c r="A93" t="s">
         <v>895</v>
       </c>
@@ -35776,7 +35785,7 @@
       <c r="I93" s="140"/>
       <c r="J93" s="140"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" hidden="1">
       <c r="A94" t="s">
         <v>895</v>
       </c>
@@ -35804,7 +35813,7 @@
       <c r="I94" s="140"/>
       <c r="J94" s="140"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" hidden="1">
       <c r="A95" t="s">
         <v>895</v>
       </c>
@@ -35830,7 +35839,7 @@
       <c r="I95" s="140"/>
       <c r="J95" s="140"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" hidden="1">
       <c r="A96" t="s">
         <v>895</v>
       </c>
@@ -35856,7 +35865,7 @@
       <c r="I96" s="140"/>
       <c r="J96" s="140"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" hidden="1">
       <c r="A97" t="s">
         <v>145</v>
       </c>
@@ -35882,7 +35891,7 @@
       <c r="I97" s="140"/>
       <c r="J97" s="140"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" hidden="1">
       <c r="A98" t="s">
         <v>145</v>
       </c>
@@ -35910,7 +35919,7 @@
       <c r="I98" s="140"/>
       <c r="J98" s="140"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" hidden="1">
       <c r="A99" t="s">
         <v>145</v>
       </c>
@@ -35936,7 +35945,7 @@
       <c r="I99" s="140"/>
       <c r="J99" s="140"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" hidden="1">
       <c r="A100" t="s">
         <v>145</v>
       </c>
@@ -35962,7 +35971,7 @@
       <c r="I100" s="140"/>
       <c r="J100" s="140"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" hidden="1">
       <c r="A101" t="s">
         <v>145</v>
       </c>
@@ -35988,7 +35997,7 @@
       <c r="I101" s="140"/>
       <c r="J101" s="140"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" hidden="1">
       <c r="A102" t="s">
         <v>145</v>
       </c>
@@ -36014,7 +36023,7 @@
       <c r="I102" s="140"/>
       <c r="J102" s="140"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" hidden="1">
       <c r="A103" t="s">
         <v>145</v>
       </c>
@@ -36092,7 +36101,7 @@
       <c r="I105" s="140"/>
       <c r="J105" s="140"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" hidden="1">
       <c r="A106" t="s">
         <v>57</v>
       </c>
@@ -36144,7 +36153,7 @@
       <c r="I107" s="140"/>
       <c r="J107" s="140"/>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" hidden="1">
       <c r="A108" t="s">
         <v>895</v>
       </c>
@@ -36173,7 +36182,7 @@
       <c r="I108" s="140"/>
       <c r="J108" s="140"/>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" hidden="1">
       <c r="A109" s="156" t="s">
         <v>895</v>
       </c>
@@ -36199,7 +36208,7 @@
       <c r="I109" s="140"/>
       <c r="J109" s="140"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" hidden="1">
       <c r="A110" s="156" t="s">
         <v>895</v>
       </c>
@@ -36225,7 +36234,7 @@
       <c r="I110" s="140"/>
       <c r="J110" s="140"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" hidden="1">
       <c r="A111" s="156" t="s">
         <v>145</v>
       </c>
@@ -36251,7 +36260,7 @@
       <c r="I111" s="140"/>
       <c r="J111" s="140"/>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" hidden="1">
       <c r="A112" s="156" t="s">
         <v>145</v>
       </c>
@@ -36304,7 +36313,7 @@
       <c r="I113" s="140"/>
       <c r="J113" s="140"/>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" hidden="1">
       <c r="A114" t="s">
         <v>145</v>
       </c>
@@ -36332,7 +36341,7 @@
       <c r="I114" s="140"/>
       <c r="J114" s="140"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" hidden="1">
       <c r="A115" t="s">
         <v>145</v>
       </c>
@@ -36358,7 +36367,7 @@
       <c r="I115" s="140"/>
       <c r="J115" s="140"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" hidden="1">
       <c r="A116" t="s">
         <v>145</v>
       </c>
@@ -36410,7 +36419,7 @@
       <c r="I117" s="140"/>
       <c r="J117" s="140"/>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" hidden="1">
       <c r="D118" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36425,7 +36434,7 @@
       <c r="I118" s="140"/>
       <c r="J118" s="140"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" hidden="1">
       <c r="D119" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36440,7 +36449,7 @@
       <c r="I119" s="140"/>
       <c r="J119" s="140"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" hidden="1">
       <c r="D120" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36455,7 +36464,7 @@
       <c r="I120" s="140"/>
       <c r="J120" s="140"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" hidden="1">
       <c r="D121" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36470,7 +36479,7 @@
       <c r="I121" s="140"/>
       <c r="J121" s="140"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" hidden="1">
       <c r="D122" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36485,7 +36494,7 @@
       <c r="I122" s="140"/>
       <c r="J122" s="140"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" hidden="1">
       <c r="D123" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36500,7 +36509,7 @@
       <c r="I123" s="140"/>
       <c r="J123" s="140"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" hidden="1">
       <c r="D124" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36515,7 +36524,7 @@
       <c r="I124" s="140"/>
       <c r="J124" s="140"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" hidden="1">
       <c r="D125" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36530,7 +36539,7 @@
       <c r="I125" s="140"/>
       <c r="J125" s="140"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" hidden="1">
       <c r="D126" s="79" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -36545,7 +36554,7 @@
       <c r="I126" s="140"/>
       <c r="J126" s="140"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" hidden="1">
       <c r="D127" s="79" t="e">
         <f t="shared" ref="D127:D158" si="6">E127*(1+$T$1)</f>
         <v>#DIV/0!</v>
@@ -36560,7 +36569,7 @@
       <c r="I127" s="140"/>
       <c r="J127" s="140"/>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" hidden="1">
       <c r="D128" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36575,7 +36584,7 @@
       <c r="I128" s="140"/>
       <c r="J128" s="140"/>
     </row>
-    <row r="129" spans="4:10">
+    <row r="129" spans="4:10" hidden="1">
       <c r="D129" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36590,7 +36599,7 @@
       <c r="I129" s="140"/>
       <c r="J129" s="140"/>
     </row>
-    <row r="130" spans="4:10">
+    <row r="130" spans="4:10" hidden="1">
       <c r="D130" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36605,7 +36614,7 @@
       <c r="I130" s="140"/>
       <c r="J130" s="140"/>
     </row>
-    <row r="131" spans="4:10">
+    <row r="131" spans="4:10" hidden="1">
       <c r="D131" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36620,7 +36629,7 @@
       <c r="I131" s="140"/>
       <c r="J131" s="140"/>
     </row>
-    <row r="132" spans="4:10">
+    <row r="132" spans="4:10" hidden="1">
       <c r="D132" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36635,7 +36644,7 @@
       <c r="I132" s="140"/>
       <c r="J132" s="140"/>
     </row>
-    <row r="133" spans="4:10">
+    <row r="133" spans="4:10" hidden="1">
       <c r="D133" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36650,7 +36659,7 @@
       <c r="I133" s="140"/>
       <c r="J133" s="140"/>
     </row>
-    <row r="134" spans="4:10">
+    <row r="134" spans="4:10" hidden="1">
       <c r="D134" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36665,7 +36674,7 @@
       <c r="I134" s="140"/>
       <c r="J134" s="140"/>
     </row>
-    <row r="135" spans="4:10">
+    <row r="135" spans="4:10" hidden="1">
       <c r="D135" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36680,7 +36689,7 @@
       <c r="I135" s="140"/>
       <c r="J135" s="140"/>
     </row>
-    <row r="136" spans="4:10">
+    <row r="136" spans="4:10" hidden="1">
       <c r="D136" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36695,7 +36704,7 @@
       <c r="I136" s="140"/>
       <c r="J136" s="140"/>
     </row>
-    <row r="137" spans="4:10">
+    <row r="137" spans="4:10" hidden="1">
       <c r="D137" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36710,7 +36719,7 @@
       <c r="I137" s="140"/>
       <c r="J137" s="140"/>
     </row>
-    <row r="138" spans="4:10">
+    <row r="138" spans="4:10" hidden="1">
       <c r="D138" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36725,7 +36734,7 @@
       <c r="I138" s="140"/>
       <c r="J138" s="140"/>
     </row>
-    <row r="139" spans="4:10">
+    <row r="139" spans="4:10" hidden="1">
       <c r="D139" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36740,7 +36749,7 @@
       <c r="I139" s="140"/>
       <c r="J139" s="140"/>
     </row>
-    <row r="140" spans="4:10">
+    <row r="140" spans="4:10" hidden="1">
       <c r="D140" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36755,7 +36764,7 @@
       <c r="I140" s="140"/>
       <c r="J140" s="140"/>
     </row>
-    <row r="141" spans="4:10">
+    <row r="141" spans="4:10" hidden="1">
       <c r="D141" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36770,7 +36779,7 @@
       <c r="I141" s="140"/>
       <c r="J141" s="140"/>
     </row>
-    <row r="142" spans="4:10">
+    <row r="142" spans="4:10" hidden="1">
       <c r="D142" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36785,7 +36794,7 @@
       <c r="I142" s="140"/>
       <c r="J142" s="140"/>
     </row>
-    <row r="143" spans="4:10">
+    <row r="143" spans="4:10" hidden="1">
       <c r="D143" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36800,7 +36809,7 @@
       <c r="I143" s="140"/>
       <c r="J143" s="140"/>
     </row>
-    <row r="144" spans="4:10">
+    <row r="144" spans="4:10" hidden="1">
       <c r="D144" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36815,7 +36824,7 @@
       <c r="I144" s="140"/>
       <c r="J144" s="140"/>
     </row>
-    <row r="145" spans="4:10">
+    <row r="145" spans="4:10" hidden="1">
       <c r="D145" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36830,7 +36839,7 @@
       <c r="I145" s="140"/>
       <c r="J145" s="140"/>
     </row>
-    <row r="146" spans="4:10">
+    <row r="146" spans="4:10" hidden="1">
       <c r="D146" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36845,7 +36854,7 @@
       <c r="I146" s="140"/>
       <c r="J146" s="140"/>
     </row>
-    <row r="147" spans="4:10">
+    <row r="147" spans="4:10" hidden="1">
       <c r="D147" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36860,7 +36869,7 @@
       <c r="I147" s="140"/>
       <c r="J147" s="140"/>
     </row>
-    <row r="148" spans="4:10">
+    <row r="148" spans="4:10" hidden="1">
       <c r="D148" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36875,7 +36884,7 @@
       <c r="I148" s="140"/>
       <c r="J148" s="140"/>
     </row>
-    <row r="149" spans="4:10">
+    <row r="149" spans="4:10" hidden="1">
       <c r="D149" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36890,7 +36899,7 @@
       <c r="I149" s="140"/>
       <c r="J149" s="140"/>
     </row>
-    <row r="150" spans="4:10">
+    <row r="150" spans="4:10" hidden="1">
       <c r="D150" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36905,7 +36914,7 @@
       <c r="I150" s="140"/>
       <c r="J150" s="140"/>
     </row>
-    <row r="151" spans="4:10">
+    <row r="151" spans="4:10" hidden="1">
       <c r="D151" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36920,7 +36929,7 @@
       <c r="I151" s="140"/>
       <c r="J151" s="140"/>
     </row>
-    <row r="152" spans="4:10">
+    <row r="152" spans="4:10" hidden="1">
       <c r="D152" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36935,7 +36944,7 @@
       <c r="I152" s="140"/>
       <c r="J152" s="140"/>
     </row>
-    <row r="153" spans="4:10">
+    <row r="153" spans="4:10" hidden="1">
       <c r="D153" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36950,7 +36959,7 @@
       <c r="I153" s="140"/>
       <c r="J153" s="140"/>
     </row>
-    <row r="154" spans="4:10">
+    <row r="154" spans="4:10" hidden="1">
       <c r="D154" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36965,7 +36974,7 @@
       <c r="I154" s="140"/>
       <c r="J154" s="140"/>
     </row>
-    <row r="155" spans="4:10">
+    <row r="155" spans="4:10" hidden="1">
       <c r="D155" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36980,7 +36989,7 @@
       <c r="I155" s="140"/>
       <c r="J155" s="140"/>
     </row>
-    <row r="156" spans="4:10">
+    <row r="156" spans="4:10" hidden="1">
       <c r="D156" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -36995,7 +37004,7 @@
       <c r="I156" s="140"/>
       <c r="J156" s="140"/>
     </row>
-    <row r="157" spans="4:10">
+    <row r="157" spans="4:10" hidden="1">
       <c r="D157" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -37010,7 +37019,7 @@
       <c r="I157" s="140"/>
       <c r="J157" s="140"/>
     </row>
-    <row r="158" spans="4:10">
+    <row r="158" spans="4:10" hidden="1">
       <c r="D158" s="79" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
@@ -37025,9 +37034,9 @@
       <c r="I158" s="140"/>
       <c r="J158" s="140"/>
     </row>
-    <row r="159" spans="4:10">
+    <row r="159" spans="4:10" hidden="1">
       <c r="D159" s="79" t="e">
-        <f t="shared" ref="D159:D190" si="8">E159*(1+$T$1)</f>
+        <f t="shared" ref="D159:D170" si="8">E159*(1+$T$1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E159" s="79" t="e">
@@ -37040,7 +37049,7 @@
       <c r="I159" s="140"/>
       <c r="J159" s="140"/>
     </row>
-    <row r="160" spans="4:10">
+    <row r="160" spans="4:10" hidden="1">
       <c r="D160" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37055,7 +37064,7 @@
       <c r="I160" s="140"/>
       <c r="J160" s="140"/>
     </row>
-    <row r="161" spans="4:10">
+    <row r="161" spans="4:10" hidden="1">
       <c r="D161" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37070,7 +37079,7 @@
       <c r="I161" s="140"/>
       <c r="J161" s="140"/>
     </row>
-    <row r="162" spans="4:10">
+    <row r="162" spans="4:10" hidden="1">
       <c r="D162" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37085,7 +37094,7 @@
       <c r="I162" s="140"/>
       <c r="J162" s="140"/>
     </row>
-    <row r="163" spans="4:10">
+    <row r="163" spans="4:10" hidden="1">
       <c r="D163" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37100,7 +37109,7 @@
       <c r="I163" s="140"/>
       <c r="J163" s="140"/>
     </row>
-    <row r="164" spans="4:10">
+    <row r="164" spans="4:10" hidden="1">
       <c r="D164" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37115,7 +37124,7 @@
       <c r="I164" s="140"/>
       <c r="J164" s="140"/>
     </row>
-    <row r="165" spans="4:10">
+    <row r="165" spans="4:10" hidden="1">
       <c r="D165" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37130,7 +37139,7 @@
       <c r="I165" s="140"/>
       <c r="J165" s="140"/>
     </row>
-    <row r="166" spans="4:10">
+    <row r="166" spans="4:10" hidden="1">
       <c r="D166" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37145,7 +37154,7 @@
       <c r="I166" s="140"/>
       <c r="J166" s="140"/>
     </row>
-    <row r="167" spans="4:10">
+    <row r="167" spans="4:10" hidden="1">
       <c r="D167" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37160,7 +37169,7 @@
       <c r="I167" s="140"/>
       <c r="J167" s="140"/>
     </row>
-    <row r="168" spans="4:10">
+    <row r="168" spans="4:10" hidden="1">
       <c r="D168" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37175,7 +37184,7 @@
       <c r="I168" s="140"/>
       <c r="J168" s="140"/>
     </row>
-    <row r="169" spans="4:10">
+    <row r="169" spans="4:10" hidden="1">
       <c r="D169" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37190,7 +37199,7 @@
       <c r="I169" s="140"/>
       <c r="J169" s="140"/>
     </row>
-    <row r="170" spans="4:10">
+    <row r="170" spans="4:10" hidden="1">
       <c r="D170" s="79" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
@@ -37205,7 +37214,7 @@
       <c r="I170" s="140"/>
       <c r="J170" s="140"/>
     </row>
-    <row r="171" spans="4:10">
+    <row r="171" spans="4:10" hidden="1">
       <c r="D171" s="79" t="e">
         <f t="shared" ref="D171:D202" si="9">E171*(1+$O$1)</f>
         <v>#DIV/0!</v>
@@ -37220,7 +37229,7 @@
       <c r="I171" s="140"/>
       <c r="J171" s="140"/>
     </row>
-    <row r="172" spans="4:10">
+    <row r="172" spans="4:10" hidden="1">
       <c r="D172" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37235,7 +37244,7 @@
       <c r="I172" s="140"/>
       <c r="J172" s="140"/>
     </row>
-    <row r="173" spans="4:10">
+    <row r="173" spans="4:10" hidden="1">
       <c r="D173" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37250,7 +37259,7 @@
       <c r="I173" s="140"/>
       <c r="J173" s="140"/>
     </row>
-    <row r="174" spans="4:10">
+    <row r="174" spans="4:10" hidden="1">
       <c r="D174" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37265,7 +37274,7 @@
       <c r="I174" s="140"/>
       <c r="J174" s="140"/>
     </row>
-    <row r="175" spans="4:10">
+    <row r="175" spans="4:10" hidden="1">
       <c r="D175" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37280,7 +37289,7 @@
       <c r="I175" s="140"/>
       <c r="J175" s="140"/>
     </row>
-    <row r="176" spans="4:10">
+    <row r="176" spans="4:10" hidden="1">
       <c r="D176" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37295,7 +37304,7 @@
       <c r="I176" s="140"/>
       <c r="J176" s="140"/>
     </row>
-    <row r="177" spans="4:10">
+    <row r="177" spans="4:10" hidden="1">
       <c r="D177" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37310,7 +37319,7 @@
       <c r="I177" s="140"/>
       <c r="J177" s="140"/>
     </row>
-    <row r="178" spans="4:10">
+    <row r="178" spans="4:10" hidden="1">
       <c r="D178" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37325,7 +37334,7 @@
       <c r="I178" s="140"/>
       <c r="J178" s="140"/>
     </row>
-    <row r="179" spans="4:10">
+    <row r="179" spans="4:10" hidden="1">
       <c r="D179" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37340,7 +37349,7 @@
       <c r="I179" s="140"/>
       <c r="J179" s="140"/>
     </row>
-    <row r="180" spans="4:10">
+    <row r="180" spans="4:10" hidden="1">
       <c r="D180" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37355,7 +37364,7 @@
       <c r="I180" s="140"/>
       <c r="J180" s="140"/>
     </row>
-    <row r="181" spans="4:10">
+    <row r="181" spans="4:10" hidden="1">
       <c r="D181" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37370,7 +37379,7 @@
       <c r="I181" s="140"/>
       <c r="J181" s="140"/>
     </row>
-    <row r="182" spans="4:10">
+    <row r="182" spans="4:10" hidden="1">
       <c r="D182" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37385,7 +37394,7 @@
       <c r="I182" s="140"/>
       <c r="J182" s="140"/>
     </row>
-    <row r="183" spans="4:10">
+    <row r="183" spans="4:10" hidden="1">
       <c r="D183" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37400,7 +37409,7 @@
       <c r="I183" s="140"/>
       <c r="J183" s="140"/>
     </row>
-    <row r="184" spans="4:10">
+    <row r="184" spans="4:10" hidden="1">
       <c r="D184" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37415,7 +37424,7 @@
       <c r="I184" s="140"/>
       <c r="J184" s="140"/>
     </row>
-    <row r="185" spans="4:10">
+    <row r="185" spans="4:10" hidden="1">
       <c r="D185" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37430,7 +37439,7 @@
       <c r="I185" s="140"/>
       <c r="J185" s="140"/>
     </row>
-    <row r="186" spans="4:10">
+    <row r="186" spans="4:10" hidden="1">
       <c r="D186" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37445,7 +37454,7 @@
       <c r="I186" s="140"/>
       <c r="J186" s="140"/>
     </row>
-    <row r="187" spans="4:10">
+    <row r="187" spans="4:10" hidden="1">
       <c r="D187" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37460,7 +37469,7 @@
       <c r="I187" s="140"/>
       <c r="J187" s="140"/>
     </row>
-    <row r="188" spans="4:10">
+    <row r="188" spans="4:10" hidden="1">
       <c r="D188" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37475,7 +37484,7 @@
       <c r="I188" s="140"/>
       <c r="J188" s="140"/>
     </row>
-    <row r="189" spans="4:10">
+    <row r="189" spans="4:10" hidden="1">
       <c r="D189" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37490,7 +37499,7 @@
       <c r="I189" s="140"/>
       <c r="J189" s="140"/>
     </row>
-    <row r="190" spans="4:10">
+    <row r="190" spans="4:10" hidden="1">
       <c r="D190" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37505,7 +37514,7 @@
       <c r="I190" s="140"/>
       <c r="J190" s="140"/>
     </row>
-    <row r="191" spans="4:10">
+    <row r="191" spans="4:10" hidden="1">
       <c r="D191" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37520,7 +37529,7 @@
       <c r="I191" s="140"/>
       <c r="J191" s="140"/>
     </row>
-    <row r="192" spans="4:10">
+    <row r="192" spans="4:10" hidden="1">
       <c r="D192" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37535,7 +37544,7 @@
       <c r="I192" s="140"/>
       <c r="J192" s="140"/>
     </row>
-    <row r="193" spans="4:10">
+    <row r="193" spans="4:10" hidden="1">
       <c r="D193" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37550,13 +37559,13 @@
       <c r="I193" s="140"/>
       <c r="J193" s="140"/>
     </row>
-    <row r="194" spans="4:10">
+    <row r="194" spans="4:10" hidden="1">
       <c r="D194" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E194" s="140" t="e">
-        <f t="shared" ref="E194:E257" si="10">AVERAGE(F194:Q194)</f>
+        <f t="shared" ref="E194:E246" si="10">AVERAGE(F194:Q194)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F194" s="140"/>
@@ -37565,7 +37574,7 @@
       <c r="I194" s="140"/>
       <c r="J194" s="140"/>
     </row>
-    <row r="195" spans="4:10">
+    <row r="195" spans="4:10" hidden="1">
       <c r="D195" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37580,7 +37589,7 @@
       <c r="I195" s="140"/>
       <c r="J195" s="140"/>
     </row>
-    <row r="196" spans="4:10">
+    <row r="196" spans="4:10" hidden="1">
       <c r="D196" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37595,7 +37604,7 @@
       <c r="I196" s="140"/>
       <c r="J196" s="140"/>
     </row>
-    <row r="197" spans="4:10">
+    <row r="197" spans="4:10" hidden="1">
       <c r="D197" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37610,7 +37619,7 @@
       <c r="I197" s="140"/>
       <c r="J197" s="140"/>
     </row>
-    <row r="198" spans="4:10">
+    <row r="198" spans="4:10" hidden="1">
       <c r="D198" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37625,7 +37634,7 @@
       <c r="I198" s="140"/>
       <c r="J198" s="140"/>
     </row>
-    <row r="199" spans="4:10">
+    <row r="199" spans="4:10" hidden="1">
       <c r="D199" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37640,7 +37649,7 @@
       <c r="I199" s="140"/>
       <c r="J199" s="140"/>
     </row>
-    <row r="200" spans="4:10">
+    <row r="200" spans="4:10" hidden="1">
       <c r="D200" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37655,7 +37664,7 @@
       <c r="I200" s="140"/>
       <c r="J200" s="140"/>
     </row>
-    <row r="201" spans="4:10">
+    <row r="201" spans="4:10" hidden="1">
       <c r="D201" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37670,7 +37679,7 @@
       <c r="I201" s="140"/>
       <c r="J201" s="140"/>
     </row>
-    <row r="202" spans="4:10">
+    <row r="202" spans="4:10" hidden="1">
       <c r="D202" s="79" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
@@ -37685,7 +37694,7 @@
       <c r="I202" s="140"/>
       <c r="J202" s="140"/>
     </row>
-    <row r="203" spans="4:10">
+    <row r="203" spans="4:10" hidden="1">
       <c r="D203" s="79" t="e">
         <f t="shared" ref="D203:D234" si="11">E203*(1+$O$1)</f>
         <v>#DIV/0!</v>
@@ -37700,7 +37709,7 @@
       <c r="I203" s="140"/>
       <c r="J203" s="140"/>
     </row>
-    <row r="204" spans="4:10">
+    <row r="204" spans="4:10" hidden="1">
       <c r="D204" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37715,7 +37724,7 @@
       <c r="I204" s="140"/>
       <c r="J204" s="140"/>
     </row>
-    <row r="205" spans="4:10">
+    <row r="205" spans="4:10" hidden="1">
       <c r="D205" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37730,7 +37739,7 @@
       <c r="I205" s="140"/>
       <c r="J205" s="140"/>
     </row>
-    <row r="206" spans="4:10">
+    <row r="206" spans="4:10" hidden="1">
       <c r="D206" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37745,7 +37754,7 @@
       <c r="I206" s="140"/>
       <c r="J206" s="140"/>
     </row>
-    <row r="207" spans="4:10">
+    <row r="207" spans="4:10" hidden="1">
       <c r="D207" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37760,7 +37769,7 @@
       <c r="I207" s="140"/>
       <c r="J207" s="140"/>
     </row>
-    <row r="208" spans="4:10">
+    <row r="208" spans="4:10" hidden="1">
       <c r="D208" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37775,7 +37784,7 @@
       <c r="I208" s="140"/>
       <c r="J208" s="140"/>
     </row>
-    <row r="209" spans="4:10">
+    <row r="209" spans="4:10" hidden="1">
       <c r="D209" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37790,7 +37799,7 @@
       <c r="I209" s="140"/>
       <c r="J209" s="140"/>
     </row>
-    <row r="210" spans="4:10">
+    <row r="210" spans="4:10" hidden="1">
       <c r="D210" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37805,7 +37814,7 @@
       <c r="I210" s="140"/>
       <c r="J210" s="140"/>
     </row>
-    <row r="211" spans="4:10">
+    <row r="211" spans="4:10" hidden="1">
       <c r="D211" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37820,7 +37829,7 @@
       <c r="I211" s="140"/>
       <c r="J211" s="140"/>
     </row>
-    <row r="212" spans="4:10">
+    <row r="212" spans="4:10" hidden="1">
       <c r="D212" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37835,7 +37844,7 @@
       <c r="I212" s="140"/>
       <c r="J212" s="140"/>
     </row>
-    <row r="213" spans="4:10">
+    <row r="213" spans="4:10" hidden="1">
       <c r="D213" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37850,7 +37859,7 @@
       <c r="I213" s="140"/>
       <c r="J213" s="140"/>
     </row>
-    <row r="214" spans="4:10">
+    <row r="214" spans="4:10" hidden="1">
       <c r="D214" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37865,7 +37874,7 @@
       <c r="I214" s="140"/>
       <c r="J214" s="140"/>
     </row>
-    <row r="215" spans="4:10">
+    <row r="215" spans="4:10" hidden="1">
       <c r="D215" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37880,7 +37889,7 @@
       <c r="I215" s="140"/>
       <c r="J215" s="140"/>
     </row>
-    <row r="216" spans="4:10">
+    <row r="216" spans="4:10" hidden="1">
       <c r="D216" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37895,7 +37904,7 @@
       <c r="I216" s="140"/>
       <c r="J216" s="140"/>
     </row>
-    <row r="217" spans="4:10">
+    <row r="217" spans="4:10" hidden="1">
       <c r="D217" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37910,7 +37919,7 @@
       <c r="I217" s="140"/>
       <c r="J217" s="140"/>
     </row>
-    <row r="218" spans="4:10">
+    <row r="218" spans="4:10" hidden="1">
       <c r="D218" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37925,7 +37934,7 @@
       <c r="I218" s="140"/>
       <c r="J218" s="140"/>
     </row>
-    <row r="219" spans="4:10">
+    <row r="219" spans="4:10" hidden="1">
       <c r="D219" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37940,7 +37949,7 @@
       <c r="I219" s="140"/>
       <c r="J219" s="140"/>
     </row>
-    <row r="220" spans="4:10">
+    <row r="220" spans="4:10" hidden="1">
       <c r="D220" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37955,7 +37964,7 @@
       <c r="I220" s="140"/>
       <c r="J220" s="140"/>
     </row>
-    <row r="221" spans="4:10">
+    <row r="221" spans="4:10" hidden="1">
       <c r="D221" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37970,7 +37979,7 @@
       <c r="I221" s="140"/>
       <c r="J221" s="140"/>
     </row>
-    <row r="222" spans="4:10">
+    <row r="222" spans="4:10" hidden="1">
       <c r="D222" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -37985,7 +37994,7 @@
       <c r="I222" s="140"/>
       <c r="J222" s="140"/>
     </row>
-    <row r="223" spans="4:10">
+    <row r="223" spans="4:10" hidden="1">
       <c r="D223" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38000,7 +38009,7 @@
       <c r="I223" s="140"/>
       <c r="J223" s="140"/>
     </row>
-    <row r="224" spans="4:10">
+    <row r="224" spans="4:10" hidden="1">
       <c r="D224" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38015,7 +38024,7 @@
       <c r="I224" s="140"/>
       <c r="J224" s="140"/>
     </row>
-    <row r="225" spans="4:10">
+    <row r="225" spans="4:10" hidden="1">
       <c r="D225" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38030,7 +38039,7 @@
       <c r="I225" s="140"/>
       <c r="J225" s="140"/>
     </row>
-    <row r="226" spans="4:10">
+    <row r="226" spans="4:10" hidden="1">
       <c r="D226" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38045,7 +38054,7 @@
       <c r="I226" s="140"/>
       <c r="J226" s="140"/>
     </row>
-    <row r="227" spans="4:10">
+    <row r="227" spans="4:10" hidden="1">
       <c r="D227" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38060,7 +38069,7 @@
       <c r="I227" s="140"/>
       <c r="J227" s="140"/>
     </row>
-    <row r="228" spans="4:10">
+    <row r="228" spans="4:10" hidden="1">
       <c r="D228" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38075,7 +38084,7 @@
       <c r="I228" s="140"/>
       <c r="J228" s="140"/>
     </row>
-    <row r="229" spans="4:10">
+    <row r="229" spans="4:10" hidden="1">
       <c r="D229" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38090,7 +38099,7 @@
       <c r="I229" s="140"/>
       <c r="J229" s="140"/>
     </row>
-    <row r="230" spans="4:10">
+    <row r="230" spans="4:10" hidden="1">
       <c r="D230" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38105,7 +38114,7 @@
       <c r="I230" s="140"/>
       <c r="J230" s="140"/>
     </row>
-    <row r="231" spans="4:10">
+    <row r="231" spans="4:10" hidden="1">
       <c r="D231" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38120,7 +38129,7 @@
       <c r="I231" s="140"/>
       <c r="J231" s="140"/>
     </row>
-    <row r="232" spans="4:10">
+    <row r="232" spans="4:10" hidden="1">
       <c r="D232" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38135,7 +38144,7 @@
       <c r="I232" s="140"/>
       <c r="J232" s="140"/>
     </row>
-    <row r="233" spans="4:10">
+    <row r="233" spans="4:10" hidden="1">
       <c r="D233" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38150,7 +38159,7 @@
       <c r="I233" s="140"/>
       <c r="J233" s="140"/>
     </row>
-    <row r="234" spans="4:10">
+    <row r="234" spans="4:10" hidden="1">
       <c r="D234" s="79" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
@@ -38165,9 +38174,9 @@
       <c r="I234" s="140"/>
       <c r="J234" s="140"/>
     </row>
-    <row r="235" spans="4:10">
+    <row r="235" spans="4:10" hidden="1">
       <c r="D235" s="79" t="e">
-        <f t="shared" ref="D235:D266" si="12">E235*(1+$O$1)</f>
+        <f t="shared" ref="D235:D246" si="12">E235*(1+$O$1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E235" s="140" t="e">
@@ -38180,7 +38189,7 @@
       <c r="I235" s="140"/>
       <c r="J235" s="140"/>
     </row>
-    <row r="236" spans="4:10">
+    <row r="236" spans="4:10" hidden="1">
       <c r="D236" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -38195,7 +38204,7 @@
       <c r="I236" s="140"/>
       <c r="J236" s="140"/>
     </row>
-    <row r="237" spans="4:10">
+    <row r="237" spans="4:10" hidden="1">
       <c r="D237" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -38210,7 +38219,7 @@
       <c r="I237" s="140"/>
       <c r="J237" s="140"/>
     </row>
-    <row r="238" spans="4:10">
+    <row r="238" spans="4:10" hidden="1">
       <c r="D238" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -38225,7 +38234,7 @@
       <c r="I238" s="140"/>
       <c r="J238" s="140"/>
     </row>
-    <row r="239" spans="4:10">
+    <row r="239" spans="4:10" hidden="1">
       <c r="D239" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -38240,7 +38249,7 @@
       <c r="I239" s="140"/>
       <c r="J239" s="140"/>
     </row>
-    <row r="240" spans="4:10">
+    <row r="240" spans="4:10" hidden="1">
       <c r="D240" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -38255,7 +38264,7 @@
       <c r="I240" s="140"/>
       <c r="J240" s="140"/>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" hidden="1">
       <c r="D241" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -38270,7 +38279,7 @@
       <c r="I241" s="140"/>
       <c r="J241" s="140"/>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" hidden="1">
       <c r="D242" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -38285,7 +38294,7 @@
       <c r="I242" s="140"/>
       <c r="J242" s="140"/>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" hidden="1">
       <c r="D243" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -38300,7 +38309,7 @@
       <c r="I243" s="140"/>
       <c r="J243" s="140"/>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" hidden="1">
       <c r="A244" s="156"/>
       <c r="D244" s="79" t="e">
         <f t="shared" si="12"/>
@@ -38316,7 +38325,7 @@
       <c r="I244" s="140"/>
       <c r="J244" s="140"/>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" hidden="1">
       <c r="A245" s="156"/>
       <c r="D245" s="79" t="e">
         <f t="shared" si="12"/>
@@ -38332,7 +38341,7 @@
       <c r="I245" s="140"/>
       <c r="J245" s="140"/>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" hidden="1">
       <c r="D246" s="79" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
@@ -52746,18 +52755,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
     <mergeCell ref="J33:L33"/>
     <mergeCell ref="M33:O33"/>
     <mergeCell ref="S27:U27"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="V17:X17"/>
     <mergeCell ref="M27:O27"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -56658,10 +56667,10 @@
       <c r="A4" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="246" t="s">
+      <c r="C4" s="244" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="248">
+      <c r="D4" s="246">
         <f>SUMPRODUCT(I4:I9, E4:E9)</f>
         <v>20.011428571428571</v>
       </c>
@@ -56701,8 +56710,8 @@
       <c r="A5" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="246"/>
-      <c r="D5" s="248"/>
+      <c r="C5" s="244"/>
+      <c r="D5" s="246"/>
       <c r="E5" s="212">
         <v>5</v>
       </c>
@@ -56739,8 +56748,8 @@
       <c r="A6" s="160" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="246"/>
-      <c r="D6" s="248"/>
+      <c r="C6" s="244"/>
+      <c r="D6" s="246"/>
       <c r="E6" s="212">
         <v>1</v>
       </c>
@@ -56770,8 +56779,8 @@
       <c r="A7" s="160" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="246"/>
-      <c r="D7" s="248"/>
+      <c r="C7" s="244"/>
+      <c r="D7" s="246"/>
       <c r="E7" s="212">
         <v>1</v>
       </c>
@@ -56805,8 +56814,8 @@
       <c r="A8" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="246"/>
-      <c r="D8" s="248"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="246"/>
       <c r="E8" s="212">
         <v>0</v>
       </c>
@@ -56840,8 +56849,8 @@
       <c r="A9" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="247"/>
-      <c r="D9" s="249"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="247"/>
       <c r="E9" s="167">
         <v>2</v>
       </c>
@@ -56896,25 +56905,25 @@
       <c r="A12" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="242" t="s">
+      <c r="F12" s="249" t="s">
         <v>166</v>
       </c>
-      <c r="G12" s="242"/>
-      <c r="H12" s="242"/>
-      <c r="I12" s="242"/>
-      <c r="J12" s="242"/>
+      <c r="G12" s="249"/>
+      <c r="H12" s="249"/>
+      <c r="I12" s="249"/>
+      <c r="J12" s="249"/>
     </row>
     <row r="13" spans="1:15" ht="19">
       <c r="A13" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="241" t="s">
+      <c r="F13" s="248" t="s">
         <v>167</v>
       </c>
-      <c r="G13" s="241"/>
-      <c r="H13" s="241"/>
-      <c r="I13" s="241"/>
-      <c r="J13" s="241"/>
+      <c r="G13" s="248"/>
+      <c r="H13" s="248"/>
+      <c r="I13" s="248"/>
+      <c r="J13" s="248"/>
       <c r="K13" s="159"/>
       <c r="L13" s="159"/>
       <c r="M13" s="159"/>
@@ -56923,13 +56932,13 @@
       <c r="A14" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="241" t="s">
+      <c r="F14" s="248" t="s">
         <v>168</v>
       </c>
-      <c r="G14" s="241"/>
-      <c r="H14" s="241"/>
-      <c r="I14" s="241"/>
-      <c r="J14" s="241"/>
+      <c r="G14" s="248"/>
+      <c r="H14" s="248"/>
+      <c r="I14" s="248"/>
+      <c r="J14" s="248"/>
       <c r="K14" s="159"/>
       <c r="L14" s="159"/>
       <c r="M14" s="159"/>
@@ -56938,28 +56947,28 @@
       <c r="A15" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="241" t="s">
+      <c r="F15" s="248" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="241"/>
-      <c r="H15" s="241"/>
-      <c r="I15" s="241"/>
-      <c r="J15" s="241"/>
-      <c r="K15" s="241"/>
-      <c r="L15" s="241"/>
-      <c r="M15" s="241"/>
+      <c r="G15" s="248"/>
+      <c r="H15" s="248"/>
+      <c r="I15" s="248"/>
+      <c r="J15" s="248"/>
+      <c r="K15" s="248"/>
+      <c r="L15" s="248"/>
+      <c r="M15" s="248"/>
     </row>
     <row r="16" spans="1:15" ht="19">
       <c r="A16" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="241" t="s">
+      <c r="F16" s="248" t="s">
         <v>170</v>
       </c>
-      <c r="G16" s="241"/>
-      <c r="H16" s="241"/>
-      <c r="I16" s="241"/>
-      <c r="J16" s="241"/>
+      <c r="G16" s="248"/>
+      <c r="H16" s="248"/>
+      <c r="I16" s="248"/>
+      <c r="J16" s="248"/>
       <c r="K16" s="159"/>
       <c r="L16" s="159"/>
       <c r="M16" s="159"/>
@@ -56968,13 +56977,13 @@
       <c r="A17" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="241" t="s">
+      <c r="F17" s="248" t="s">
         <v>171</v>
       </c>
-      <c r="G17" s="241"/>
-      <c r="H17" s="241"/>
-      <c r="I17" s="241"/>
-      <c r="J17" s="241"/>
+      <c r="G17" s="248"/>
+      <c r="H17" s="248"/>
+      <c r="I17" s="248"/>
+      <c r="J17" s="248"/>
       <c r="K17" s="159"/>
       <c r="L17" s="159"/>
       <c r="M17" s="159"/>
@@ -57024,10 +57033,10 @@
       <c r="A20" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="243" t="s">
+      <c r="B20" s="241" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="243" t="s">
+      <c r="C20" s="241" t="s">
         <v>179</v>
       </c>
       <c r="D20" s="87"/>
@@ -57095,12 +57104,12 @@
       <c r="A21" s="159" t="s">
         <v>190</v>
       </c>
-      <c r="B21" s="243"/>
-      <c r="C21" s="243"/>
-      <c r="D21" s="244" t="s">
+      <c r="B21" s="241"/>
+      <c r="C21" s="241"/>
+      <c r="D21" s="242" t="s">
         <v>191</v>
       </c>
-      <c r="E21" s="245"/>
+      <c r="E21" s="243"/>
       <c r="F21" s="74"/>
       <c r="G21" s="74"/>
       <c r="H21" s="74"/>
@@ -57533,10 +57542,10 @@
       <c r="A30" s="160" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="244" t="s">
+      <c r="D30" s="242" t="s">
         <v>247</v>
       </c>
-      <c r="E30" s="245"/>
+      <c r="E30" s="243"/>
       <c r="F30" s="74"/>
       <c r="G30" s="74"/>
       <c r="H30" s="74"/>
@@ -59183,18 +59192,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F15:M15"/>
+    <mergeCell ref="F16:J16"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="C4:C9"/>
     <mergeCell ref="D4:D9"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F15:M15"/>
-    <mergeCell ref="F16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -59354,10 +59363,10 @@
       <c r="A4" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="246" t="s">
+      <c r="D4" s="244" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="248">
+      <c r="E4" s="246">
         <f>SUMPRODUCT(F4:F9, J4:J9)</f>
         <v>53.968672586474355</v>
       </c>
@@ -59388,8 +59397,8 @@
       <c r="A5" s="160" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="246"/>
-      <c r="E5" s="248"/>
+      <c r="D5" s="244"/>
+      <c r="E5" s="246"/>
       <c r="F5" s="212">
         <v>7.0000219999999969</v>
       </c>
@@ -59417,8 +59426,8 @@
       <c r="A6" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="246"/>
-      <c r="E6" s="248"/>
+      <c r="D6" s="244"/>
+      <c r="E6" s="246"/>
       <c r="F6" s="212">
         <v>5</v>
       </c>
@@ -59446,8 +59455,8 @@
       <c r="A7" s="160" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="246"/>
-      <c r="E7" s="248"/>
+      <c r="D7" s="244"/>
+      <c r="E7" s="246"/>
       <c r="F7" s="212">
         <v>6</v>
       </c>
@@ -59475,8 +59484,8 @@
       <c r="A8" s="160" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="246"/>
-      <c r="E8" s="248"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="246"/>
       <c r="F8" s="212">
         <v>0</v>
       </c>
@@ -59504,8 +59513,8 @@
       <c r="A9" s="160" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="247"/>
-      <c r="E9" s="249"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="247"/>
       <c r="F9" s="167">
         <v>6</v>
       </c>
@@ -59566,13 +59575,13 @@
       <c r="A13" s="160" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="241" t="s">
+      <c r="G13" s="248" t="s">
         <v>167</v>
       </c>
-      <c r="H13" s="241"/>
-      <c r="I13" s="241"/>
-      <c r="J13" s="241"/>
-      <c r="K13" s="241"/>
+      <c r="H13" s="248"/>
+      <c r="I13" s="248"/>
+      <c r="J13" s="248"/>
+      <c r="K13" s="248"/>
       <c r="L13" s="159"/>
       <c r="M13" s="159"/>
       <c r="N13" s="159"/>
@@ -59581,13 +59590,13 @@
       <c r="A14" s="160" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="241" t="s">
+      <c r="G14" s="248" t="s">
         <v>168</v>
       </c>
-      <c r="H14" s="241"/>
-      <c r="I14" s="241"/>
-      <c r="J14" s="241"/>
-      <c r="K14" s="241"/>
+      <c r="H14" s="248"/>
+      <c r="I14" s="248"/>
+      <c r="J14" s="248"/>
+      <c r="K14" s="248"/>
       <c r="L14" s="159"/>
       <c r="M14" s="159"/>
       <c r="N14" s="159"/>
@@ -59596,28 +59605,28 @@
       <c r="A15" s="160" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="241" t="s">
+      <c r="G15" s="248" t="s">
         <v>169</v>
       </c>
-      <c r="H15" s="241"/>
-      <c r="I15" s="241"/>
-      <c r="J15" s="241"/>
-      <c r="K15" s="241"/>
-      <c r="L15" s="241"/>
-      <c r="M15" s="241"/>
-      <c r="N15" s="241"/>
+      <c r="H15" s="248"/>
+      <c r="I15" s="248"/>
+      <c r="J15" s="248"/>
+      <c r="K15" s="248"/>
+      <c r="L15" s="248"/>
+      <c r="M15" s="248"/>
+      <c r="N15" s="248"/>
     </row>
     <row r="16" spans="1:14" ht="19">
       <c r="A16" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="241" t="s">
+      <c r="G16" s="248" t="s">
         <v>170</v>
       </c>
-      <c r="H16" s="241"/>
-      <c r="I16" s="241"/>
-      <c r="J16" s="241"/>
-      <c r="K16" s="241"/>
+      <c r="H16" s="248"/>
+      <c r="I16" s="248"/>
+      <c r="J16" s="248"/>
+      <c r="K16" s="248"/>
       <c r="L16" s="159"/>
       <c r="M16" s="159"/>
       <c r="N16" s="159"/>
@@ -59626,13 +59635,13 @@
       <c r="A17" s="160" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="241" t="s">
+      <c r="G17" s="248" t="s">
         <v>171</v>
       </c>
-      <c r="H17" s="241"/>
-      <c r="I17" s="241"/>
-      <c r="J17" s="241"/>
-      <c r="K17" s="241"/>
+      <c r="H17" s="248"/>
+      <c r="I17" s="248"/>
+      <c r="J17" s="248"/>
+      <c r="K17" s="248"/>
       <c r="L17" s="159"/>
       <c r="M17" s="159"/>
       <c r="N17" s="159"/>
@@ -59688,10 +59697,10 @@
       <c r="A20" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="243" t="s">
+      <c r="B20" s="241" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="243" t="s">
+      <c r="C20" s="241" t="s">
         <v>179</v>
       </c>
       <c r="F20" s="71" t="s">
@@ -59810,12 +59819,12 @@
       <c r="A21" s="160" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="243"/>
-      <c r="C21" s="243"/>
-      <c r="D21" s="244" t="s">
+      <c r="B21" s="241"/>
+      <c r="C21" s="241"/>
+      <c r="D21" s="242" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="245"/>
+      <c r="E21" s="243"/>
     </row>
     <row r="22" spans="1:42" ht="87" thickTop="1" thickBot="1">
       <c r="A22" s="160" t="s">
@@ -59901,10 +59910,10 @@
       <c r="A29" s="160" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="244" t="s">
+      <c r="D29" s="242" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="245"/>
+      <c r="E29" s="243"/>
     </row>
     <row r="30" spans="1:42" ht="53" thickTop="1" thickBot="1">
       <c r="A30" s="160" t="s">
@@ -60262,18 +60271,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:N15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G13:K13"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D4:D9"/>
     <mergeCell ref="E4:E9"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:N15"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -60445,10 +60454,10 @@
       <c r="A4" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="246" t="s">
+      <c r="D4" s="244" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="248">
+      <c r="E4" s="246">
         <f>SUMPRODUCT(J4:J9, F4:F9)</f>
         <v>34.552586765086765</v>
       </c>
@@ -60481,8 +60490,8 @@
       <c r="A5" s="160" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="246"/>
-      <c r="E5" s="248"/>
+      <c r="D5" s="244"/>
+      <c r="E5" s="246"/>
       <c r="F5" s="212">
         <v>10</v>
       </c>
@@ -60512,8 +60521,8 @@
       <c r="A6" s="160" t="s">
         <v>351</v>
       </c>
-      <c r="D6" s="246"/>
-      <c r="E6" s="248"/>
+      <c r="D6" s="244"/>
+      <c r="E6" s="246"/>
       <c r="F6" s="212">
         <v>3</v>
       </c>
@@ -60543,8 +60552,8 @@
       <c r="A7" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="246"/>
-      <c r="E7" s="248"/>
+      <c r="D7" s="244"/>
+      <c r="E7" s="246"/>
       <c r="F7" s="212">
         <v>3</v>
       </c>
@@ -60574,8 +60583,8 @@
       <c r="A8" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="246"/>
-      <c r="E8" s="248"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="246"/>
       <c r="F8" s="212">
         <v>1</v>
       </c>
@@ -60605,8 +60614,8 @@
       <c r="A9" s="160" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="247"/>
-      <c r="E9" s="249"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="247"/>
       <c r="F9" s="167">
         <v>3</v>
       </c>
@@ -60656,13 +60665,13 @@
       <c r="A12" s="160" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="251" t="s">
+      <c r="G12" s="253" t="s">
         <v>353</v>
       </c>
-      <c r="H12" s="251"/>
-      <c r="I12" s="251"/>
-      <c r="J12" s="251"/>
-      <c r="K12" s="251"/>
+      <c r="H12" s="253"/>
+      <c r="I12" s="253"/>
+      <c r="J12" s="253"/>
+      <c r="K12" s="253"/>
       <c r="L12" s="211"/>
       <c r="M12" s="211"/>
     </row>
@@ -60670,13 +60679,13 @@
       <c r="A13" s="160" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="241" t="s">
+      <c r="G13" s="248" t="s">
         <v>167</v>
       </c>
-      <c r="H13" s="241"/>
-      <c r="I13" s="241"/>
-      <c r="J13" s="241"/>
-      <c r="K13" s="241"/>
+      <c r="H13" s="248"/>
+      <c r="I13" s="248"/>
+      <c r="J13" s="248"/>
+      <c r="K13" s="248"/>
       <c r="L13" s="210"/>
       <c r="M13" s="210"/>
       <c r="N13" s="159"/>
@@ -60687,13 +60696,13 @@
       <c r="A14" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="241" t="s">
+      <c r="G14" s="248" t="s">
         <v>168</v>
       </c>
-      <c r="H14" s="241"/>
-      <c r="I14" s="241"/>
-      <c r="J14" s="241"/>
-      <c r="K14" s="241"/>
+      <c r="H14" s="248"/>
+      <c r="I14" s="248"/>
+      <c r="J14" s="248"/>
+      <c r="K14" s="248"/>
       <c r="L14" s="210"/>
       <c r="M14" s="210"/>
       <c r="N14" s="159"/>
@@ -60704,30 +60713,30 @@
       <c r="A15" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="241" t="s">
+      <c r="G15" s="248" t="s">
         <v>169</v>
       </c>
-      <c r="H15" s="241"/>
-      <c r="I15" s="241"/>
-      <c r="J15" s="241"/>
-      <c r="K15" s="241"/>
-      <c r="L15" s="241"/>
-      <c r="M15" s="241"/>
-      <c r="N15" s="241"/>
-      <c r="O15" s="241"/>
-      <c r="P15" s="241"/>
+      <c r="H15" s="248"/>
+      <c r="I15" s="248"/>
+      <c r="J15" s="248"/>
+      <c r="K15" s="248"/>
+      <c r="L15" s="248"/>
+      <c r="M15" s="248"/>
+      <c r="N15" s="248"/>
+      <c r="O15" s="248"/>
+      <c r="P15" s="248"/>
     </row>
     <row r="16" spans="1:31" ht="19">
       <c r="A16" s="160" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="241" t="s">
+      <c r="G16" s="248" t="s">
         <v>170</v>
       </c>
-      <c r="H16" s="241"/>
-      <c r="I16" s="241"/>
-      <c r="J16" s="241"/>
-      <c r="K16" s="241"/>
+      <c r="H16" s="248"/>
+      <c r="I16" s="248"/>
+      <c r="J16" s="248"/>
+      <c r="K16" s="248"/>
       <c r="L16" s="210"/>
       <c r="M16" s="210"/>
       <c r="N16" s="159"/>
@@ -60743,13 +60752,13 @@
       <c r="A17" s="160" t="s">
         <v>121</v>
       </c>
-      <c r="G17" s="241" t="s">
+      <c r="G17" s="248" t="s">
         <v>171</v>
       </c>
-      <c r="H17" s="241"/>
-      <c r="I17" s="241"/>
-      <c r="J17" s="241"/>
-      <c r="K17" s="241"/>
+      <c r="H17" s="248"/>
+      <c r="I17" s="248"/>
+      <c r="J17" s="248"/>
+      <c r="K17" s="248"/>
       <c r="L17" s="210"/>
       <c r="M17" s="210" t="s">
         <v>354</v>
@@ -60835,10 +60844,10 @@
       <c r="A21" s="160" t="s">
         <v>125</v>
       </c>
-      <c r="B21" s="243" t="s">
+      <c r="B21" s="241" t="s">
         <v>178</v>
       </c>
-      <c r="C21" s="243" t="s">
+      <c r="C21" s="241" t="s">
         <v>179</v>
       </c>
       <c r="F21" s="87" t="s">
@@ -60957,12 +60966,12 @@
       <c r="A22" s="160" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="243"/>
-      <c r="C22" s="243"/>
-      <c r="D22" s="244" t="s">
+      <c r="B22" s="241"/>
+      <c r="C22" s="241"/>
+      <c r="D22" s="242" t="s">
         <v>371</v>
       </c>
-      <c r="E22" s="245"/>
+      <c r="E22" s="243"/>
       <c r="F22" s="74"/>
       <c r="G22" s="74"/>
       <c r="H22" s="74"/>
@@ -61620,10 +61629,10 @@
       <c r="A28" s="160" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="244" t="s">
+      <c r="D28" s="242" t="s">
         <v>436</v>
       </c>
-      <c r="E28" s="245"/>
+      <c r="E28" s="243"/>
       <c r="F28" s="74"/>
       <c r="G28" s="74"/>
       <c r="H28" s="74"/>
@@ -62666,10 +62675,10 @@
       <c r="A39" s="160" t="s">
         <v>109</v>
       </c>
-      <c r="D39" s="252" t="s">
+      <c r="D39" s="251" t="s">
         <v>505</v>
       </c>
-      <c r="E39" s="253"/>
+      <c r="E39" s="252"/>
       <c r="F39" s="74">
         <v>1</v>
       </c>
@@ -63400,11 +63409,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
     <mergeCell ref="G16:K16"/>
     <mergeCell ref="G17:K17"/>
     <mergeCell ref="G15:P15"/>
@@ -63413,6 +63417,11 @@
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G14:K14"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -63557,13 +63566,13 @@
       <c r="A3" s="158" t="s">
         <v>154</v>
       </c>
-      <c r="F3" s="256" t="s">
+      <c r="F3" s="254" t="s">
         <v>511</v>
       </c>
-      <c r="G3" s="256"/>
-      <c r="H3" s="256"/>
-      <c r="I3" s="256"/>
-      <c r="J3" s="256"/>
+      <c r="G3" s="254"/>
+      <c r="H3" s="254"/>
+      <c r="I3" s="254"/>
+      <c r="J3" s="254"/>
       <c r="O3">
         <f>COUNT($E$24:$E$29)</f>
         <v>6</v>
@@ -63573,13 +63582,13 @@
       <c r="A4" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="241" t="s">
+      <c r="F4" s="248" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="241"/>
-      <c r="H4" s="241"/>
-      <c r="I4" s="241"/>
-      <c r="J4" s="241"/>
+      <c r="G4" s="248"/>
+      <c r="H4" s="248"/>
+      <c r="I4" s="248"/>
+      <c r="J4" s="248"/>
       <c r="K4" s="159"/>
       <c r="L4" s="159"/>
       <c r="M4" s="159"/>
@@ -63592,13 +63601,13 @@
       <c r="A5" s="160" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="241" t="s">
+      <c r="F5" s="248" t="s">
         <v>512</v>
       </c>
-      <c r="G5" s="241"/>
-      <c r="H5" s="241"/>
-      <c r="I5" s="241"/>
-      <c r="J5" s="241"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="248"/>
+      <c r="J5" s="248"/>
       <c r="K5" s="159"/>
       <c r="L5" s="159"/>
       <c r="M5" s="159"/>
@@ -63611,16 +63620,16 @@
       <c r="A6" s="160" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="241" t="s">
+      <c r="F6" s="248" t="s">
         <v>169</v>
       </c>
-      <c r="G6" s="241"/>
-      <c r="H6" s="241"/>
-      <c r="I6" s="241"/>
-      <c r="J6" s="241"/>
-      <c r="K6" s="241"/>
-      <c r="L6" s="241"/>
-      <c r="M6" s="241"/>
+      <c r="G6" s="248"/>
+      <c r="H6" s="248"/>
+      <c r="I6" s="248"/>
+      <c r="J6" s="248"/>
+      <c r="K6" s="248"/>
+      <c r="L6" s="248"/>
+      <c r="M6" s="248"/>
       <c r="O6" t="b">
         <f>$E$24&lt;=3</f>
         <v>0</v>
@@ -63630,13 +63639,13 @@
       <c r="A7" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="241" t="s">
+      <c r="F7" s="248" t="s">
         <v>170</v>
       </c>
-      <c r="G7" s="241"/>
-      <c r="H7" s="241"/>
-      <c r="I7" s="241"/>
-      <c r="J7" s="241"/>
+      <c r="G7" s="248"/>
+      <c r="H7" s="248"/>
+      <c r="I7" s="248"/>
+      <c r="J7" s="248"/>
       <c r="K7" s="159"/>
       <c r="L7" s="159"/>
       <c r="M7" s="159"/>
@@ -63649,13 +63658,13 @@
       <c r="A8" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="241" t="s">
+      <c r="F8" s="248" t="s">
         <v>171</v>
       </c>
-      <c r="G8" s="241"/>
-      <c r="H8" s="241"/>
-      <c r="I8" s="241"/>
-      <c r="J8" s="241"/>
+      <c r="G8" s="248"/>
+      <c r="H8" s="248"/>
+      <c r="I8" s="248"/>
+      <c r="J8" s="248"/>
       <c r="K8" s="159"/>
       <c r="L8" s="159"/>
       <c r="M8" s="159"/>
@@ -63707,7 +63716,7 @@
       <c r="A12" s="160" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="254" t="s">
+      <c r="B12" s="255" t="s">
         <v>513</v>
       </c>
       <c r="C12" s="202"/>
@@ -63739,11 +63748,11 @@
       <c r="A13" s="160" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="255"/>
-      <c r="C13" s="246" t="s">
+      <c r="B13" s="256"/>
+      <c r="C13" s="244" t="s">
         <v>514</v>
       </c>
-      <c r="D13" s="248">
+      <c r="D13" s="246">
         <f>SUMPRODUCT(E13:E18, I13:I18)</f>
         <v>30.132308987308988</v>
       </c>
@@ -63778,9 +63787,9 @@
       <c r="A14" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="255"/>
-      <c r="C14" s="246"/>
-      <c r="D14" s="248"/>
+      <c r="B14" s="256"/>
+      <c r="C14" s="244"/>
+      <c r="D14" s="246"/>
       <c r="E14" s="212">
         <v>7</v>
       </c>
@@ -63812,9 +63821,9 @@
       <c r="A15" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="255"/>
-      <c r="C15" s="246"/>
-      <c r="D15" s="248"/>
+      <c r="B15" s="256"/>
+      <c r="C15" s="244"/>
+      <c r="D15" s="246"/>
       <c r="E15" s="212">
         <v>1</v>
       </c>
@@ -63846,9 +63855,9 @@
       <c r="A16" s="160" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="255"/>
-      <c r="C16" s="246"/>
-      <c r="D16" s="248"/>
+      <c r="B16" s="256"/>
+      <c r="C16" s="244"/>
+      <c r="D16" s="246"/>
       <c r="E16" s="212">
         <v>3</v>
       </c>
@@ -63880,9 +63889,9 @@
       <c r="A17" s="160" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="255"/>
-      <c r="C17" s="246"/>
-      <c r="D17" s="248"/>
+      <c r="B17" s="256"/>
+      <c r="C17" s="244"/>
+      <c r="D17" s="246"/>
       <c r="E17" s="212">
         <v>3</v>
       </c>
@@ -63914,9 +63923,9 @@
       <c r="A18" s="160" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="255"/>
-      <c r="C18" s="247"/>
-      <c r="D18" s="249"/>
+      <c r="B18" s="256"/>
+      <c r="C18" s="245"/>
+      <c r="D18" s="247"/>
       <c r="E18" s="167">
         <v>3</v>
       </c>
@@ -64009,7 +64018,7 @@
       <c r="A23" s="160" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="254" t="s">
+      <c r="B23" s="255" t="s">
         <v>515</v>
       </c>
       <c r="C23" s="202"/>
@@ -64037,11 +64046,11 @@
       <c r="A24" s="159" t="s">
         <v>424</v>
       </c>
-      <c r="B24" s="255"/>
-      <c r="C24" s="246" t="s">
+      <c r="B24" s="256"/>
+      <c r="C24" s="244" t="s">
         <v>514</v>
       </c>
-      <c r="D24" s="248">
+      <c r="D24" s="246">
         <f>SUMPRODUCT(I24:I29, E24:E29)</f>
         <v>48.233104765604764</v>
       </c>
@@ -64073,9 +64082,9 @@
       <c r="A25" s="160" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="255"/>
-      <c r="C25" s="246"/>
-      <c r="D25" s="248"/>
+      <c r="B25" s="256"/>
+      <c r="C25" s="244"/>
+      <c r="D25" s="246"/>
       <c r="E25" s="212">
         <v>11</v>
       </c>
@@ -64104,9 +64113,9 @@
       <c r="A26" s="159" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="255"/>
-      <c r="C26" s="246"/>
-      <c r="D26" s="248"/>
+      <c r="B26" s="256"/>
+      <c r="C26" s="244"/>
+      <c r="D26" s="246"/>
       <c r="E26" s="212">
         <v>3</v>
       </c>
@@ -64135,9 +64144,9 @@
       <c r="A27" s="160" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="255"/>
-      <c r="C27" s="246"/>
-      <c r="D27" s="248"/>
+      <c r="B27" s="256"/>
+      <c r="C27" s="244"/>
+      <c r="D27" s="246"/>
       <c r="E27" s="212">
         <v>5</v>
       </c>
@@ -64166,9 +64175,9 @@
       <c r="A28" s="160" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="255"/>
-      <c r="C28" s="246"/>
-      <c r="D28" s="248"/>
+      <c r="B28" s="256"/>
+      <c r="C28" s="244"/>
+      <c r="D28" s="246"/>
       <c r="E28" s="212">
         <v>4</v>
       </c>
@@ -64197,9 +64206,9 @@
       <c r="A29" s="160" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="255"/>
-      <c r="C29" s="247"/>
-      <c r="D29" s="249"/>
+      <c r="B29" s="256"/>
+      <c r="C29" s="245"/>
+      <c r="D29" s="247"/>
       <c r="E29" s="167">
         <v>4</v>
       </c>
@@ -64262,7 +64271,7 @@
       <c r="A33" s="160" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="254" t="s">
+      <c r="B33" s="255" t="s">
         <v>516</v>
       </c>
       <c r="C33" s="202"/>
@@ -64290,11 +64299,11 @@
       <c r="A34" s="160" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="255"/>
-      <c r="C34" s="246" t="s">
+      <c r="B34" s="256"/>
+      <c r="C34" s="244" t="s">
         <v>514</v>
       </c>
-      <c r="D34" s="248">
+      <c r="D34" s="246">
         <f>SUMPRODUCT(E34:E39, I34:I39)</f>
         <v>19.419383579383581</v>
       </c>
@@ -64326,9 +64335,9 @@
       <c r="A35" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="255"/>
-      <c r="C35" s="246"/>
-      <c r="D35" s="248"/>
+      <c r="B35" s="256"/>
+      <c r="C35" s="244"/>
+      <c r="D35" s="246"/>
       <c r="E35" s="212">
         <v>7</v>
       </c>
@@ -64357,9 +64366,9 @@
       <c r="A36" s="160" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="255"/>
-      <c r="C36" s="246"/>
-      <c r="D36" s="248"/>
+      <c r="B36" s="256"/>
+      <c r="C36" s="244"/>
+      <c r="D36" s="246"/>
       <c r="E36" s="212">
         <v>1</v>
       </c>
@@ -64388,9 +64397,9 @@
       <c r="A37" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="255"/>
-      <c r="C37" s="246"/>
-      <c r="D37" s="248"/>
+      <c r="B37" s="256"/>
+      <c r="C37" s="244"/>
+      <c r="D37" s="246"/>
       <c r="E37" s="212">
         <v>1</v>
       </c>
@@ -64419,9 +64428,9 @@
       <c r="A38" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="255"/>
-      <c r="C38" s="246"/>
-      <c r="D38" s="248"/>
+      <c r="B38" s="256"/>
+      <c r="C38" s="244"/>
+      <c r="D38" s="246"/>
       <c r="E38" s="212">
         <v>1</v>
       </c>
@@ -64450,9 +64459,9 @@
       <c r="A39" s="160" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="255"/>
-      <c r="C39" s="247"/>
-      <c r="D39" s="249"/>
+      <c r="B39" s="256"/>
+      <c r="C39" s="245"/>
+      <c r="D39" s="247"/>
       <c r="E39" s="167">
         <v>2</v>
       </c>
@@ -64492,7 +64501,7 @@
       <c r="A42" s="160" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="254" t="s">
+      <c r="B42" s="255" t="s">
         <v>518</v>
       </c>
       <c r="C42" s="202"/>
@@ -64520,11 +64529,11 @@
       <c r="A43" s="160" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="255"/>
-      <c r="C43" s="246" t="s">
+      <c r="B43" s="256"/>
+      <c r="C43" s="244" t="s">
         <v>514</v>
       </c>
-      <c r="D43" s="248">
+      <c r="D43" s="246">
         <f>SUMPRODUCT(E43:E48, I43:I48)</f>
         <v>18.360681818181821</v>
       </c>
@@ -64556,9 +64565,9 @@
       <c r="A44" s="160" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="255"/>
-      <c r="C44" s="246"/>
-      <c r="D44" s="248"/>
+      <c r="B44" s="256"/>
+      <c r="C44" s="244"/>
+      <c r="D44" s="246"/>
       <c r="E44" s="212">
         <v>0</v>
       </c>
@@ -64587,9 +64596,9 @@
       <c r="A45" s="160" t="s">
         <v>130</v>
       </c>
-      <c r="B45" s="255"/>
-      <c r="C45" s="246"/>
-      <c r="D45" s="248"/>
+      <c r="B45" s="256"/>
+      <c r="C45" s="244"/>
+      <c r="D45" s="246"/>
       <c r="E45" s="212">
         <v>0</v>
       </c>
@@ -64618,9 +64627,9 @@
       <c r="A46" s="160" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="255"/>
-      <c r="C46" s="246"/>
-      <c r="D46" s="248"/>
+      <c r="B46" s="256"/>
+      <c r="C46" s="244"/>
+      <c r="D46" s="246"/>
       <c r="E46" s="212">
         <v>0</v>
       </c>
@@ -64649,9 +64658,9 @@
       <c r="A47" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="255"/>
-      <c r="C47" s="246"/>
-      <c r="D47" s="248"/>
+      <c r="B47" s="256"/>
+      <c r="C47" s="244"/>
+      <c r="D47" s="246"/>
       <c r="E47" s="212">
         <v>2</v>
       </c>
@@ -64680,9 +64689,9 @@
       <c r="A48" s="160" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="255"/>
-      <c r="C48" s="247"/>
-      <c r="D48" s="249"/>
+      <c r="B48" s="256"/>
+      <c r="C48" s="245"/>
+      <c r="D48" s="247"/>
       <c r="E48" s="167">
         <v>1</v>
       </c>
@@ -64877,10 +64886,10 @@
       </c>
       <c r="B53" s="209"/>
       <c r="C53" s="209"/>
-      <c r="D53" s="244" t="s">
+      <c r="D53" s="242" t="s">
         <v>522</v>
       </c>
-      <c r="E53" s="245"/>
+      <c r="E53" s="243"/>
       <c r="F53" s="74"/>
       <c r="G53" s="74"/>
       <c r="H53" s="74"/>
@@ -65465,10 +65474,10 @@
       <c r="A59" s="160" t="s">
         <v>142</v>
       </c>
-      <c r="D59" s="244" t="s">
+      <c r="D59" s="242" t="s">
         <v>530</v>
       </c>
-      <c r="E59" s="245"/>
+      <c r="E59" s="243"/>
       <c r="F59" s="74"/>
       <c r="G59" s="74"/>
       <c r="H59" s="74"/>
@@ -66516,13 +66525,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="F6:M6"/>
-    <mergeCell ref="F7:J7"/>
     <mergeCell ref="B42:B48"/>
     <mergeCell ref="C43:C48"/>
     <mergeCell ref="D43:D48"/>
@@ -66536,6 +66538,13 @@
     <mergeCell ref="B23:B29"/>
     <mergeCell ref="C24:C29"/>
     <mergeCell ref="D24:D29"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="F6:M6"/>
+    <mergeCell ref="F7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -69173,52 +69182,52 @@
       <c r="D2" s="143" t="s">
         <v>568</v>
       </c>
-      <c r="E2" s="263" t="s">
+      <c r="E2" s="264" t="s">
         <v>569</v>
       </c>
-      <c r="F2" s="263"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="264" t="s">
+      <c r="F2" s="264"/>
+      <c r="G2" s="264"/>
+      <c r="H2" s="265" t="s">
         <v>570</v>
       </c>
-      <c r="I2" s="264"/>
-      <c r="J2" s="264"/>
-      <c r="K2" s="265" t="s">
+      <c r="I2" s="265"/>
+      <c r="J2" s="265"/>
+      <c r="K2" s="266" t="s">
         <v>571</v>
       </c>
-      <c r="L2" s="265"/>
-      <c r="M2" s="265"/>
-      <c r="N2" s="266" t="s">
+      <c r="L2" s="266"/>
+      <c r="M2" s="266"/>
+      <c r="N2" s="267" t="s">
         <v>572</v>
       </c>
-      <c r="O2" s="266"/>
-      <c r="P2" s="266"/>
-      <c r="Q2" s="267" t="s">
+      <c r="O2" s="267"/>
+      <c r="P2" s="267"/>
+      <c r="Q2" s="268" t="s">
         <v>573</v>
       </c>
-      <c r="R2" s="267"/>
-      <c r="S2" s="267"/>
-      <c r="T2" s="268" t="s">
+      <c r="R2" s="268"/>
+      <c r="S2" s="268"/>
+      <c r="T2" s="269" t="s">
         <v>574</v>
       </c>
-      <c r="U2" s="268"/>
-      <c r="V2" s="268"/>
-      <c r="W2" s="269" t="s">
+      <c r="U2" s="269"/>
+      <c r="V2" s="269"/>
+      <c r="W2" s="260" t="s">
         <v>575</v>
       </c>
-      <c r="X2" s="269"/>
-      <c r="Y2" s="269"/>
-      <c r="Z2" s="259" t="s">
+      <c r="X2" s="260"/>
+      <c r="Y2" s="260"/>
+      <c r="Z2" s="261" t="s">
         <v>576</v>
       </c>
-      <c r="AA2" s="259"/>
-      <c r="AB2" s="260"/>
+      <c r="AA2" s="261"/>
+      <c r="AB2" s="262"/>
     </row>
     <row r="3" spans="2:28">
       <c r="C3" s="145" t="s">
         <v>577</v>
       </c>
-      <c r="D3" s="261" t="s">
+      <c r="D3" s="259" t="s">
         <v>309</v>
       </c>
       <c r="AB3" s="115"/>
@@ -69227,14 +69236,14 @@
       <c r="C4" s="146" t="s">
         <v>578</v>
       </c>
-      <c r="D4" s="261"/>
+      <c r="D4" s="259"/>
       <c r="AB4" s="115"/>
     </row>
     <row r="5" spans="2:28">
       <c r="C5" s="148" t="s">
         <v>579</v>
       </c>
-      <c r="D5" s="262"/>
+      <c r="D5" s="263"/>
       <c r="E5" s="97"/>
       <c r="F5" s="97"/>
       <c r="G5" s="97"/>
@@ -69264,7 +69273,7 @@
       <c r="C6" s="145" t="s">
         <v>577</v>
       </c>
-      <c r="D6" s="261" t="s">
+      <c r="D6" s="259" t="s">
         <v>309</v>
       </c>
       <c r="AB6" s="115"/>
@@ -69273,14 +69282,14 @@
       <c r="C7" s="146" t="s">
         <v>578</v>
       </c>
-      <c r="D7" s="261"/>
+      <c r="D7" s="259"/>
       <c r="AB7" s="115"/>
     </row>
     <row r="8" spans="2:28">
       <c r="C8" s="148" t="s">
         <v>579</v>
       </c>
-      <c r="D8" s="262"/>
+      <c r="D8" s="263"/>
       <c r="E8" s="97"/>
       <c r="F8" s="97"/>
       <c r="G8" s="97"/>
@@ -69310,7 +69319,7 @@
       <c r="C9" s="145" t="s">
         <v>577</v>
       </c>
-      <c r="D9" s="261" t="s">
+      <c r="D9" s="259" t="s">
         <v>309</v>
       </c>
       <c r="AB9" s="115"/>
@@ -69319,21 +69328,21 @@
       <c r="C10" s="146" t="s">
         <v>578</v>
       </c>
-      <c r="D10" s="261"/>
+      <c r="D10" s="259"/>
       <c r="AB10" s="115"/>
     </row>
     <row r="11" spans="2:28">
       <c r="C11" s="147" t="s">
         <v>579</v>
       </c>
-      <c r="D11" s="261"/>
+      <c r="D11" s="259"/>
       <c r="AB11" s="115"/>
     </row>
     <row r="12" spans="2:28">
       <c r="C12" s="145" t="s">
         <v>577</v>
       </c>
-      <c r="D12" s="261" t="s">
+      <c r="D12" s="259" t="s">
         <v>41</v>
       </c>
       <c r="AB12" s="115"/>
@@ -69342,21 +69351,21 @@
       <c r="C13" s="146" t="s">
         <v>578</v>
       </c>
-      <c r="D13" s="261"/>
+      <c r="D13" s="259"/>
       <c r="AB13" s="115"/>
     </row>
     <row r="14" spans="2:28">
       <c r="C14" s="147" t="s">
         <v>579</v>
       </c>
-      <c r="D14" s="261"/>
+      <c r="D14" s="259"/>
       <c r="AB14" s="115"/>
     </row>
     <row r="15" spans="2:28">
       <c r="C15" s="145" t="s">
         <v>577</v>
       </c>
-      <c r="D15" s="261" t="s">
+      <c r="D15" s="259" t="s">
         <v>580</v>
       </c>
       <c r="AB15" s="115"/>
@@ -69365,21 +69374,21 @@
       <c r="C16" s="146" t="s">
         <v>578</v>
       </c>
-      <c r="D16" s="261"/>
+      <c r="D16" s="259"/>
       <c r="AB16" s="115"/>
     </row>
     <row r="17" spans="3:28">
       <c r="C17" s="147" t="s">
         <v>579</v>
       </c>
-      <c r="D17" s="261"/>
+      <c r="D17" s="259"/>
       <c r="AB17" s="115"/>
     </row>
     <row r="18" spans="3:28">
       <c r="C18" s="145" t="s">
         <v>577</v>
       </c>
-      <c r="D18" s="261" t="s">
+      <c r="D18" s="259" t="s">
         <v>54</v>
       </c>
       <c r="AB18" s="115"/>
@@ -69388,21 +69397,21 @@
       <c r="C19" s="146" t="s">
         <v>578</v>
       </c>
-      <c r="D19" s="261"/>
+      <c r="D19" s="259"/>
       <c r="AB19" s="115"/>
     </row>
     <row r="20" spans="3:28">
       <c r="C20" s="147" t="s">
         <v>579</v>
       </c>
-      <c r="D20" s="261"/>
+      <c r="D20" s="259"/>
       <c r="AB20" s="115"/>
     </row>
     <row r="21" spans="3:28">
       <c r="C21" s="145" t="s">
         <v>577</v>
       </c>
-      <c r="D21" s="261" t="s">
+      <c r="D21" s="259" t="s">
         <v>33</v>
       </c>
       <c r="AB21" s="115"/>
@@ -69411,21 +69420,21 @@
       <c r="C22" s="146" t="s">
         <v>578</v>
       </c>
-      <c r="D22" s="261"/>
+      <c r="D22" s="259"/>
       <c r="AB22" s="115"/>
     </row>
     <row r="23" spans="3:28">
       <c r="C23" s="147" t="s">
         <v>579</v>
       </c>
-      <c r="D23" s="261"/>
+      <c r="D23" s="259"/>
       <c r="AB23" s="115"/>
     </row>
     <row r="24" spans="3:28">
       <c r="C24" s="145" t="s">
         <v>577</v>
       </c>
-      <c r="D24" s="261" t="s">
+      <c r="D24" s="259" t="s">
         <v>28</v>
       </c>
       <c r="AB24" s="115"/>
@@ -69434,14 +69443,14 @@
       <c r="C25" s="146" t="s">
         <v>578</v>
       </c>
-      <c r="D25" s="261"/>
+      <c r="D25" s="259"/>
       <c r="AB25" s="115"/>
     </row>
     <row r="26" spans="3:28">
       <c r="C26" s="147" t="s">
         <v>579</v>
       </c>
-      <c r="D26" s="261"/>
+      <c r="D26" s="259"/>
       <c r="AB26" s="115"/>
     </row>
     <row r="27" spans="3:28">
@@ -69650,11 +69659,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="W2:Y2"/>
     <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="D6:D8"/>
@@ -69666,6 +69670,11 @@
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="T2:V2"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="W2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>